<commit_message>
docs: tambah logo dan gantt chart
</commit_message>
<xml_diff>
--- a/Gantt Chart.xlsx
+++ b/Gantt Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vertex42.com\Documents\VERTEX42\TEMPLATES\TEMPLATE - Gantt Chart\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\punch\Documents\GitHub\warawiriweb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD68E8B-A387-4742-AE63-A0C7101476C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{963D25DB-5EFA-4DFD-B2E6-A7A172356C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="23955" windowHeight="14385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="prevWBS" localSheetId="0">GanttChart!$A1048576</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">GanttChart!$A$1:$BN$37</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">GanttChart!$A$1:$BN$30</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">GanttChartPro!$A$1:$C$47</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">GanttChart!$4:$7</definedName>
     <definedName name="valuevx">42.314159</definedName>
@@ -453,17 +453,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="142">
-  <si>
-    <t>[Company Name]</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="162">
   <si>
     <t>WBS</t>
   </si>
   <si>
-    <t>[Project Name] Project Schedule</t>
-  </si>
-  <si>
     <t>TEMPLATE ROWS</t>
   </si>
   <si>
@@ -489,9 +483,6 @@
   </si>
   <si>
     <t>[Task]</t>
-  </si>
-  <si>
-    <t>[Name]</t>
   </si>
   <si>
     <t>Changing the Color of the Bars in the Gantt Chart</t>
@@ -1488,9 +1479,6 @@
     </r>
   </si>
   <si>
-    <t>[Sub-task]</t>
-  </si>
-  <si>
     <t>Method 2 will work, but Excel will split/fracture/duplicate conditional formatting rules rather than merging the rules. This can cause inefficiencies in very large and heavily modified files.</t>
   </si>
   <si>
@@ -1537,6 +1525,78 @@
       </rPr>
       <t>+1</t>
     </r>
+  </si>
+  <si>
+    <t>Wara Wiri Tour Website Project Schedule</t>
+  </si>
+  <si>
+    <t>PT. HAMID JAYA ABADI</t>
+  </si>
+  <si>
+    <t>Geizka Rozilia Ruicosta</t>
+  </si>
+  <si>
+    <t>Initiation</t>
+  </si>
+  <si>
+    <t>Costa</t>
+  </si>
+  <si>
+    <t>Client Meeting 1</t>
+  </si>
+  <si>
+    <t>Project Charter</t>
+  </si>
+  <si>
+    <t>Devi</t>
+  </si>
+  <si>
+    <t>Logo</t>
+  </si>
+  <si>
+    <t>Rauli</t>
+  </si>
+  <si>
+    <t>SKPL / SRS</t>
+  </si>
+  <si>
+    <t>Design &amp; Typography</t>
+  </si>
+  <si>
+    <t>SKPL / SRS (rev)</t>
+  </si>
+  <si>
+    <t>Project Charter (rev)</t>
+  </si>
+  <si>
+    <t>Dandy</t>
+  </si>
+  <si>
+    <t>Initiation 2</t>
+  </si>
+  <si>
+    <t>Design &amp; Typography (rev)</t>
+  </si>
+  <si>
+    <t>Navbar Mockup</t>
+  </si>
+  <si>
+    <t>Initiation &amp; Web Build 1</t>
+  </si>
+  <si>
+    <t>Navbar &amp; Home Frontend</t>
+  </si>
+  <si>
+    <t>Dewi</t>
+  </si>
+  <si>
+    <t>About Us Frontend</t>
+  </si>
+  <si>
+    <t>Joy</t>
+  </si>
+  <si>
+    <t>Home &amp; About Us Mockup</t>
   </si>
 </sst>
 </file>
@@ -2485,7 +2545,7 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="173">
+  <cellXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -2801,9 +2861,6 @@
     <xf numFmtId="0" fontId="47" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -2887,24 +2944,7 @@
     </xf>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="34" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2912,14 +2952,52 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="45" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="34" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="47" fillId="25" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="47" fillId="26" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="47" fillId="26" borderId="0" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="54" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -2967,7 +3045,33 @@
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="43" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="7">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -3748,11 +3852,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BN44"/>
+  <dimension ref="A1:BN37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="AY13" sqref="AY13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3772,47 +3876,47 @@
   <sheetData>
     <row r="1" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="124" t="s">
-        <v>2</v>
+        <v>138</v>
       </c>
       <c r="B1" s="46"/>
       <c r="C1" s="46"/>
       <c r="D1" s="46"/>
       <c r="E1" s="46"/>
       <c r="F1" s="46"/>
-      <c r="I1" s="131"/>
-      <c r="K1" s="168" t="s">
-        <v>82</v>
-      </c>
-      <c r="L1" s="168"/>
-      <c r="M1" s="168"/>
-      <c r="N1" s="168"/>
-      <c r="O1" s="168"/>
-      <c r="P1" s="168"/>
-      <c r="Q1" s="168"/>
-      <c r="R1" s="168"/>
-      <c r="S1" s="168"/>
-      <c r="T1" s="168"/>
-      <c r="U1" s="168"/>
-      <c r="V1" s="168"/>
-      <c r="W1" s="168"/>
-      <c r="X1" s="168"/>
-      <c r="Y1" s="168"/>
-      <c r="Z1" s="168"/>
-      <c r="AA1" s="168"/>
-      <c r="AB1" s="168"/>
-      <c r="AC1" s="168"/>
-      <c r="AD1" s="168"/>
-      <c r="AE1" s="168"/>
+      <c r="I1" s="130"/>
+      <c r="K1" s="162" t="s">
+        <v>79</v>
+      </c>
+      <c r="L1" s="162"/>
+      <c r="M1" s="162"/>
+      <c r="N1" s="162"/>
+      <c r="O1" s="162"/>
+      <c r="P1" s="162"/>
+      <c r="Q1" s="162"/>
+      <c r="R1" s="162"/>
+      <c r="S1" s="162"/>
+      <c r="T1" s="162"/>
+      <c r="U1" s="162"/>
+      <c r="V1" s="162"/>
+      <c r="W1" s="162"/>
+      <c r="X1" s="162"/>
+      <c r="Y1" s="162"/>
+      <c r="Z1" s="162"/>
+      <c r="AA1" s="162"/>
+      <c r="AB1" s="162"/>
+      <c r="AC1" s="162"/>
+      <c r="AD1" s="162"/>
+      <c r="AE1" s="162"/>
     </row>
     <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="51" t="s">
-        <v>0</v>
+        <v>139</v>
       </c>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
       <c r="D2" s="33"/>
-      <c r="E2" s="159"/>
-      <c r="F2" s="159"/>
+      <c r="E2" s="158"/>
+      <c r="F2" s="158"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:66" ht="14.25" x14ac:dyDescent="0.2">
@@ -3845,196 +3949,198 @@
     <row r="4" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="109"/>
       <c r="B4" s="113" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4" s="170">
-        <v>43129</v>
-      </c>
-      <c r="D4" s="170"/>
-      <c r="E4" s="170"/>
+        <v>76</v>
+      </c>
+      <c r="C4" s="167">
+        <v>45194</v>
+      </c>
+      <c r="D4" s="167"/>
+      <c r="E4" s="167"/>
       <c r="F4" s="110"/>
       <c r="G4" s="113" t="s">
-        <v>78</v>
-      </c>
-      <c r="H4" s="128">
+        <v>75</v>
+      </c>
+      <c r="H4" s="127">
         <v>1</v>
       </c>
       <c r="I4" s="111"/>
       <c r="J4" s="49"/>
-      <c r="K4" s="162" t="str">
+      <c r="K4" s="164" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="L4" s="163"/>
-      <c r="M4" s="163"/>
-      <c r="N4" s="163"/>
-      <c r="O4" s="163"/>
-      <c r="P4" s="163"/>
-      <c r="Q4" s="164"/>
-      <c r="R4" s="162" t="str">
+      <c r="L4" s="165"/>
+      <c r="M4" s="165"/>
+      <c r="N4" s="165"/>
+      <c r="O4" s="165"/>
+      <c r="P4" s="165"/>
+      <c r="Q4" s="166"/>
+      <c r="R4" s="164" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="S4" s="163"/>
-      <c r="T4" s="163"/>
-      <c r="U4" s="163"/>
-      <c r="V4" s="163"/>
-      <c r="W4" s="163"/>
-      <c r="X4" s="164"/>
-      <c r="Y4" s="162" t="str">
+      <c r="S4" s="165"/>
+      <c r="T4" s="165"/>
+      <c r="U4" s="165"/>
+      <c r="V4" s="165"/>
+      <c r="W4" s="165"/>
+      <c r="X4" s="166"/>
+      <c r="Y4" s="164" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="Z4" s="163"/>
-      <c r="AA4" s="163"/>
-      <c r="AB4" s="163"/>
-      <c r="AC4" s="163"/>
-      <c r="AD4" s="163"/>
-      <c r="AE4" s="164"/>
-      <c r="AF4" s="162" t="str">
+      <c r="Z4" s="165"/>
+      <c r="AA4" s="165"/>
+      <c r="AB4" s="165"/>
+      <c r="AC4" s="165"/>
+      <c r="AD4" s="165"/>
+      <c r="AE4" s="166"/>
+      <c r="AF4" s="164" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AG4" s="163"/>
-      <c r="AH4" s="163"/>
-      <c r="AI4" s="163"/>
-      <c r="AJ4" s="163"/>
-      <c r="AK4" s="163"/>
-      <c r="AL4" s="164"/>
-      <c r="AM4" s="162" t="str">
+      <c r="AG4" s="165"/>
+      <c r="AH4" s="165"/>
+      <c r="AI4" s="165"/>
+      <c r="AJ4" s="165"/>
+      <c r="AK4" s="165"/>
+      <c r="AL4" s="166"/>
+      <c r="AM4" s="164" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AN4" s="163"/>
-      <c r="AO4" s="163"/>
-      <c r="AP4" s="163"/>
-      <c r="AQ4" s="163"/>
-      <c r="AR4" s="163"/>
-      <c r="AS4" s="164"/>
-      <c r="AT4" s="162" t="str">
+      <c r="AN4" s="165"/>
+      <c r="AO4" s="165"/>
+      <c r="AP4" s="165"/>
+      <c r="AQ4" s="165"/>
+      <c r="AR4" s="165"/>
+      <c r="AS4" s="166"/>
+      <c r="AT4" s="164" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AU4" s="163"/>
-      <c r="AV4" s="163"/>
-      <c r="AW4" s="163"/>
-      <c r="AX4" s="163"/>
-      <c r="AY4" s="163"/>
-      <c r="AZ4" s="164"/>
-      <c r="BA4" s="162" t="str">
+      <c r="AU4" s="165"/>
+      <c r="AV4" s="165"/>
+      <c r="AW4" s="165"/>
+      <c r="AX4" s="165"/>
+      <c r="AY4" s="165"/>
+      <c r="AZ4" s="166"/>
+      <c r="BA4" s="164" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="BB4" s="163"/>
-      <c r="BC4" s="163"/>
-      <c r="BD4" s="163"/>
-      <c r="BE4" s="163"/>
-      <c r="BF4" s="163"/>
-      <c r="BG4" s="164"/>
-      <c r="BH4" s="162" t="str">
+      <c r="BB4" s="165"/>
+      <c r="BC4" s="165"/>
+      <c r="BD4" s="165"/>
+      <c r="BE4" s="165"/>
+      <c r="BF4" s="165"/>
+      <c r="BG4" s="166"/>
+      <c r="BH4" s="164" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BI4" s="163"/>
-      <c r="BJ4" s="163"/>
-      <c r="BK4" s="163"/>
-      <c r="BL4" s="163"/>
-      <c r="BM4" s="163"/>
-      <c r="BN4" s="164"/>
+      <c r="BI4" s="165"/>
+      <c r="BJ4" s="165"/>
+      <c r="BK4" s="165"/>
+      <c r="BL4" s="165"/>
+      <c r="BM4" s="165"/>
+      <c r="BN4" s="166"/>
     </row>
     <row r="5" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="109"/>
       <c r="B5" s="113" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" s="169"/>
-      <c r="D5" s="169"/>
-      <c r="E5" s="169"/>
+        <v>77</v>
+      </c>
+      <c r="C5" s="163" t="s">
+        <v>140</v>
+      </c>
+      <c r="D5" s="163"/>
+      <c r="E5" s="163"/>
       <c r="F5" s="112"/>
       <c r="G5" s="112"/>
       <c r="H5" s="112"/>
       <c r="I5" s="112"/>
       <c r="J5" s="49"/>
-      <c r="K5" s="165">
+      <c r="K5" s="168">
         <f>K6</f>
-        <v>43129</v>
-      </c>
-      <c r="L5" s="166"/>
-      <c r="M5" s="166"/>
-      <c r="N5" s="166"/>
-      <c r="O5" s="166"/>
-      <c r="P5" s="166"/>
-      <c r="Q5" s="167"/>
-      <c r="R5" s="165">
+        <v>45194</v>
+      </c>
+      <c r="L5" s="169"/>
+      <c r="M5" s="169"/>
+      <c r="N5" s="169"/>
+      <c r="O5" s="169"/>
+      <c r="P5" s="169"/>
+      <c r="Q5" s="170"/>
+      <c r="R5" s="168">
         <f>R6</f>
-        <v>43136</v>
-      </c>
-      <c r="S5" s="166"/>
-      <c r="T5" s="166"/>
-      <c r="U5" s="166"/>
-      <c r="V5" s="166"/>
-      <c r="W5" s="166"/>
-      <c r="X5" s="167"/>
-      <c r="Y5" s="165">
+        <v>45201</v>
+      </c>
+      <c r="S5" s="169"/>
+      <c r="T5" s="169"/>
+      <c r="U5" s="169"/>
+      <c r="V5" s="169"/>
+      <c r="W5" s="169"/>
+      <c r="X5" s="170"/>
+      <c r="Y5" s="168">
         <f>Y6</f>
-        <v>43143</v>
-      </c>
-      <c r="Z5" s="166"/>
-      <c r="AA5" s="166"/>
-      <c r="AB5" s="166"/>
-      <c r="AC5" s="166"/>
-      <c r="AD5" s="166"/>
-      <c r="AE5" s="167"/>
-      <c r="AF5" s="165">
+        <v>45208</v>
+      </c>
+      <c r="Z5" s="169"/>
+      <c r="AA5" s="169"/>
+      <c r="AB5" s="169"/>
+      <c r="AC5" s="169"/>
+      <c r="AD5" s="169"/>
+      <c r="AE5" s="170"/>
+      <c r="AF5" s="168">
         <f>AF6</f>
-        <v>43150</v>
-      </c>
-      <c r="AG5" s="166"/>
-      <c r="AH5" s="166"/>
-      <c r="AI5" s="166"/>
-      <c r="AJ5" s="166"/>
-      <c r="AK5" s="166"/>
-      <c r="AL5" s="167"/>
-      <c r="AM5" s="165">
+        <v>45215</v>
+      </c>
+      <c r="AG5" s="169"/>
+      <c r="AH5" s="169"/>
+      <c r="AI5" s="169"/>
+      <c r="AJ5" s="169"/>
+      <c r="AK5" s="169"/>
+      <c r="AL5" s="170"/>
+      <c r="AM5" s="168">
         <f>AM6</f>
-        <v>43157</v>
-      </c>
-      <c r="AN5" s="166"/>
-      <c r="AO5" s="166"/>
-      <c r="AP5" s="166"/>
-      <c r="AQ5" s="166"/>
-      <c r="AR5" s="166"/>
-      <c r="AS5" s="167"/>
-      <c r="AT5" s="165">
+        <v>45222</v>
+      </c>
+      <c r="AN5" s="169"/>
+      <c r="AO5" s="169"/>
+      <c r="AP5" s="169"/>
+      <c r="AQ5" s="169"/>
+      <c r="AR5" s="169"/>
+      <c r="AS5" s="170"/>
+      <c r="AT5" s="168">
         <f>AT6</f>
-        <v>43164</v>
-      </c>
-      <c r="AU5" s="166"/>
-      <c r="AV5" s="166"/>
-      <c r="AW5" s="166"/>
-      <c r="AX5" s="166"/>
-      <c r="AY5" s="166"/>
-      <c r="AZ5" s="167"/>
-      <c r="BA5" s="165">
+        <v>45229</v>
+      </c>
+      <c r="AU5" s="169"/>
+      <c r="AV5" s="169"/>
+      <c r="AW5" s="169"/>
+      <c r="AX5" s="169"/>
+      <c r="AY5" s="169"/>
+      <c r="AZ5" s="170"/>
+      <c r="BA5" s="168">
         <f>BA6</f>
-        <v>43171</v>
-      </c>
-      <c r="BB5" s="166"/>
-      <c r="BC5" s="166"/>
-      <c r="BD5" s="166"/>
-      <c r="BE5" s="166"/>
-      <c r="BF5" s="166"/>
-      <c r="BG5" s="167"/>
-      <c r="BH5" s="165">
+        <v>45236</v>
+      </c>
+      <c r="BB5" s="169"/>
+      <c r="BC5" s="169"/>
+      <c r="BD5" s="169"/>
+      <c r="BE5" s="169"/>
+      <c r="BF5" s="169"/>
+      <c r="BG5" s="170"/>
+      <c r="BH5" s="168">
         <f>BH6</f>
-        <v>43178</v>
-      </c>
-      <c r="BI5" s="166"/>
-      <c r="BJ5" s="166"/>
-      <c r="BK5" s="166"/>
-      <c r="BL5" s="166"/>
-      <c r="BM5" s="166"/>
-      <c r="BN5" s="167"/>
+        <v>45243</v>
+      </c>
+      <c r="BI5" s="169"/>
+      <c r="BJ5" s="169"/>
+      <c r="BK5" s="169"/>
+      <c r="BL5" s="169"/>
+      <c r="BM5" s="169"/>
+      <c r="BN5" s="170"/>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A6" s="48"/>
@@ -4049,256 +4155,256 @@
       <c r="J6" s="49"/>
       <c r="K6" s="91">
         <f>C4-WEEKDAY(C4,1)+2+7*(H4-1)</f>
-        <v>43129</v>
+        <v>45194</v>
       </c>
       <c r="L6" s="82">
         <f t="shared" ref="L6:AQ6" si="0">K6+1</f>
-        <v>43130</v>
+        <v>45195</v>
       </c>
       <c r="M6" s="82">
         <f t="shared" si="0"/>
-        <v>43131</v>
+        <v>45196</v>
       </c>
       <c r="N6" s="82">
         <f t="shared" si="0"/>
-        <v>43132</v>
+        <v>45197</v>
       </c>
       <c r="O6" s="82">
         <f t="shared" si="0"/>
-        <v>43133</v>
+        <v>45198</v>
       </c>
       <c r="P6" s="82">
         <f t="shared" si="0"/>
-        <v>43134</v>
+        <v>45199</v>
       </c>
       <c r="Q6" s="92">
         <f t="shared" si="0"/>
-        <v>43135</v>
+        <v>45200</v>
       </c>
       <c r="R6" s="91">
         <f t="shared" si="0"/>
-        <v>43136</v>
+        <v>45201</v>
       </c>
       <c r="S6" s="82">
         <f t="shared" si="0"/>
-        <v>43137</v>
+        <v>45202</v>
       </c>
       <c r="T6" s="82">
         <f t="shared" si="0"/>
-        <v>43138</v>
+        <v>45203</v>
       </c>
       <c r="U6" s="82">
         <f t="shared" si="0"/>
-        <v>43139</v>
+        <v>45204</v>
       </c>
       <c r="V6" s="82">
         <f t="shared" si="0"/>
-        <v>43140</v>
+        <v>45205</v>
       </c>
       <c r="W6" s="82">
         <f t="shared" si="0"/>
-        <v>43141</v>
+        <v>45206</v>
       </c>
       <c r="X6" s="92">
         <f t="shared" si="0"/>
-        <v>43142</v>
+        <v>45207</v>
       </c>
       <c r="Y6" s="91">
         <f t="shared" si="0"/>
-        <v>43143</v>
+        <v>45208</v>
       </c>
       <c r="Z6" s="82">
         <f t="shared" si="0"/>
-        <v>43144</v>
+        <v>45209</v>
       </c>
       <c r="AA6" s="82">
         <f t="shared" si="0"/>
-        <v>43145</v>
+        <v>45210</v>
       </c>
       <c r="AB6" s="82">
         <f t="shared" si="0"/>
-        <v>43146</v>
+        <v>45211</v>
       </c>
       <c r="AC6" s="82">
         <f t="shared" si="0"/>
-        <v>43147</v>
+        <v>45212</v>
       </c>
       <c r="AD6" s="82">
         <f t="shared" si="0"/>
-        <v>43148</v>
+        <v>45213</v>
       </c>
       <c r="AE6" s="92">
         <f t="shared" si="0"/>
-        <v>43149</v>
+        <v>45214</v>
       </c>
       <c r="AF6" s="91">
         <f t="shared" si="0"/>
-        <v>43150</v>
+        <v>45215</v>
       </c>
       <c r="AG6" s="82">
         <f t="shared" si="0"/>
-        <v>43151</v>
+        <v>45216</v>
       </c>
       <c r="AH6" s="82">
         <f t="shared" si="0"/>
-        <v>43152</v>
+        <v>45217</v>
       </c>
       <c r="AI6" s="82">
         <f t="shared" si="0"/>
-        <v>43153</v>
+        <v>45218</v>
       </c>
       <c r="AJ6" s="82">
         <f t="shared" si="0"/>
-        <v>43154</v>
+        <v>45219</v>
       </c>
       <c r="AK6" s="82">
         <f t="shared" si="0"/>
-        <v>43155</v>
+        <v>45220</v>
       </c>
       <c r="AL6" s="92">
         <f t="shared" si="0"/>
-        <v>43156</v>
+        <v>45221</v>
       </c>
       <c r="AM6" s="91">
         <f t="shared" si="0"/>
-        <v>43157</v>
+        <v>45222</v>
       </c>
       <c r="AN6" s="82">
         <f t="shared" si="0"/>
-        <v>43158</v>
+        <v>45223</v>
       </c>
       <c r="AO6" s="82">
         <f t="shared" si="0"/>
-        <v>43159</v>
+        <v>45224</v>
       </c>
       <c r="AP6" s="82">
         <f t="shared" si="0"/>
-        <v>43160</v>
+        <v>45225</v>
       </c>
       <c r="AQ6" s="82">
         <f t="shared" si="0"/>
-        <v>43161</v>
+        <v>45226</v>
       </c>
       <c r="AR6" s="82">
         <f t="shared" ref="AR6:BN6" si="1">AQ6+1</f>
-        <v>43162</v>
+        <v>45227</v>
       </c>
       <c r="AS6" s="92">
         <f t="shared" si="1"/>
-        <v>43163</v>
+        <v>45228</v>
       </c>
       <c r="AT6" s="91">
         <f t="shared" si="1"/>
-        <v>43164</v>
+        <v>45229</v>
       </c>
       <c r="AU6" s="82">
         <f t="shared" si="1"/>
-        <v>43165</v>
+        <v>45230</v>
       </c>
       <c r="AV6" s="82">
         <f t="shared" si="1"/>
-        <v>43166</v>
+        <v>45231</v>
       </c>
       <c r="AW6" s="82">
         <f t="shared" si="1"/>
-        <v>43167</v>
+        <v>45232</v>
       </c>
       <c r="AX6" s="82">
         <f t="shared" si="1"/>
-        <v>43168</v>
+        <v>45233</v>
       </c>
       <c r="AY6" s="82">
         <f t="shared" si="1"/>
-        <v>43169</v>
+        <v>45234</v>
       </c>
       <c r="AZ6" s="92">
         <f t="shared" si="1"/>
-        <v>43170</v>
+        <v>45235</v>
       </c>
       <c r="BA6" s="91">
         <f t="shared" si="1"/>
-        <v>43171</v>
+        <v>45236</v>
       </c>
       <c r="BB6" s="82">
         <f t="shared" si="1"/>
-        <v>43172</v>
+        <v>45237</v>
       </c>
       <c r="BC6" s="82">
         <f t="shared" si="1"/>
-        <v>43173</v>
+        <v>45238</v>
       </c>
       <c r="BD6" s="82">
         <f t="shared" si="1"/>
-        <v>43174</v>
+        <v>45239</v>
       </c>
       <c r="BE6" s="82">
         <f t="shared" si="1"/>
-        <v>43175</v>
+        <v>45240</v>
       </c>
       <c r="BF6" s="82">
         <f t="shared" si="1"/>
-        <v>43176</v>
+        <v>45241</v>
       </c>
       <c r="BG6" s="92">
         <f t="shared" si="1"/>
-        <v>43177</v>
+        <v>45242</v>
       </c>
       <c r="BH6" s="91">
         <f t="shared" si="1"/>
-        <v>43178</v>
+        <v>45243</v>
       </c>
       <c r="BI6" s="82">
         <f t="shared" si="1"/>
-        <v>43179</v>
+        <v>45244</v>
       </c>
       <c r="BJ6" s="82">
         <f t="shared" si="1"/>
-        <v>43180</v>
+        <v>45245</v>
       </c>
       <c r="BK6" s="82">
         <f t="shared" si="1"/>
-        <v>43181</v>
+        <v>45246</v>
       </c>
       <c r="BL6" s="82">
         <f t="shared" si="1"/>
-        <v>43182</v>
+        <v>45247</v>
       </c>
       <c r="BM6" s="82">
         <f t="shared" si="1"/>
-        <v>43183</v>
+        <v>45248</v>
       </c>
       <c r="BN6" s="92">
         <f t="shared" si="1"/>
-        <v>43184</v>
+        <v>45249</v>
       </c>
     </row>
     <row r="7" spans="1:66" s="123" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="115" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7" s="116" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="117" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="118" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="119" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="119" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="117" t="s">
+      <c r="G7" s="117" t="s">
         <v>71</v>
       </c>
-      <c r="D7" s="118" t="s">
-        <v>77</v>
-      </c>
-      <c r="E7" s="119" t="s">
+      <c r="H7" s="117" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="119" t="s">
+      <c r="I7" s="117" t="s">
         <v>73</v>
-      </c>
-      <c r="G7" s="117" t="s">
-        <v>74</v>
-      </c>
-      <c r="H7" s="117" t="s">
-        <v>75</v>
-      </c>
-      <c r="I7" s="117" t="s">
-        <v>76</v>
       </c>
       <c r="J7" s="117"/>
       <c r="K7" s="120" t="str">
@@ -4532,20 +4638,24 @@
         <v>1</v>
       </c>
       <c r="B8" s="84" t="s">
-        <v>10</v>
+        <v>141</v>
       </c>
       <c r="C8" s="85"/>
       <c r="D8" s="86"/>
-      <c r="E8" s="87"/>
-      <c r="F8" s="114" t="str">
+      <c r="E8" s="87">
+        <v>45194</v>
+      </c>
+      <c r="F8" s="114">
         <f>IF(ISBLANK(E8)," - ",IF(G8=0,E8,E8+G8-1))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G8" s="88"/>
+        <v>45198</v>
+      </c>
+      <c r="G8" s="88">
+        <v>5</v>
+      </c>
       <c r="H8" s="89"/>
-      <c r="I8" s="90" t="str">
-        <f t="shared" ref="I8:I37" si="4">IF(OR(F8=0,E8=0)," - ",NETWORKDAYS(E8,F8))</f>
-        <v xml:space="preserve"> - </v>
+      <c r="I8" s="90">
+        <f t="shared" ref="I8:I30" si="4">IF(OR(F8=0,E8=0)," - ",NETWORKDAYS(E8,F8))</f>
+        <v>5</v>
       </c>
       <c r="J8" s="93"/>
       <c r="K8" s="105"/>
@@ -4607,32 +4717,32 @@
     </row>
     <row r="9" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="59" t="str">
-        <f t="shared" ref="A9:A17" si="5">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A9:A11" si="5">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.1</v>
       </c>
       <c r="B9" s="125" t="s">
-        <v>11</v>
+        <v>143</v>
       </c>
       <c r="C9" s="60" t="s">
-        <v>12</v>
+        <v>142</v>
       </c>
       <c r="D9" s="126"/>
       <c r="E9" s="99">
-        <v>43129</v>
+        <v>45194</v>
       </c>
       <c r="F9" s="100">
         <f>IF(ISBLANK(E9)," - ",IF(G9=0,E9,E9+G9-1))</f>
-        <v>43133</v>
+        <v>45194</v>
       </c>
       <c r="G9" s="61">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H9" s="62">
         <v>1</v>
       </c>
       <c r="I9" s="63">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J9" s="94"/>
       <c r="K9" s="106"/>
@@ -4698,21 +4808,24 @@
         <v>1.2</v>
       </c>
       <c r="B10" s="125" t="s">
-        <v>11</v>
+        <v>144</v>
+      </c>
+      <c r="C10" s="60" t="s">
+        <v>145</v>
       </c>
       <c r="D10" s="126"/>
       <c r="E10" s="99">
-        <v>43134</v>
+        <v>45195</v>
       </c>
       <c r="F10" s="100">
-        <f t="shared" ref="F10:F35" si="6">IF(ISBLANK(E10)," - ",IF(G10=0,E10,E10+G10-1))</f>
-        <v>43138</v>
+        <f t="shared" ref="F10:F28" si="6">IF(ISBLANK(E10)," - ",IF(G10=0,E10,E10+G10-1))</f>
+        <v>45197</v>
       </c>
       <c r="G10" s="61">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H10" s="62">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="I10" s="63">
         <f t="shared" si="4"/>
@@ -4782,25 +4895,28 @@
         <v>1.3</v>
       </c>
       <c r="B11" s="125" t="s">
-        <v>11</v>
+        <v>148</v>
+      </c>
+      <c r="C11" s="60" t="s">
+        <v>145</v>
       </c>
       <c r="D11" s="126"/>
       <c r="E11" s="99">
-        <v>43139</v>
+        <f>F10+1</f>
+        <v>45198</v>
       </c>
       <c r="F11" s="100">
         <f t="shared" si="6"/>
-        <v>43142</v>
+        <v>45198</v>
       </c>
       <c r="G11" s="61">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H11" s="62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="63">
-        <f t="shared" si="4"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J11" s="94"/>
       <c r="K11" s="106"/>
@@ -4860,115 +4976,117 @@
       <c r="BM11" s="106"/>
       <c r="BN11" s="106"/>
     </row>
-    <row r="12" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A12" s="59" t="str">
-        <f t="shared" si="5"/>
-        <v>1.4</v>
-      </c>
-      <c r="B12" s="125" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="126"/>
-      <c r="E12" s="99">
-        <v>43132</v>
-      </c>
-      <c r="F12" s="100">
-        <f t="shared" si="6"/>
-        <v>43135</v>
-      </c>
-      <c r="G12" s="61">
-        <v>4</v>
-      </c>
-      <c r="H12" s="62">
-        <v>0.75</v>
-      </c>
-      <c r="I12" s="63">
-        <f t="shared" si="4"/>
+    <row r="12" spans="1:66" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="52" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>2</v>
       </c>
-      <c r="J12" s="94"/>
-      <c r="K12" s="106"/>
-      <c r="L12" s="106"/>
-      <c r="M12" s="106"/>
-      <c r="N12" s="106"/>
-      <c r="O12" s="106"/>
-      <c r="P12" s="106"/>
-      <c r="Q12" s="106"/>
-      <c r="R12" s="106"/>
-      <c r="S12" s="106"/>
-      <c r="T12" s="106"/>
-      <c r="U12" s="106"/>
-      <c r="V12" s="106"/>
-      <c r="W12" s="106"/>
-      <c r="X12" s="106"/>
-      <c r="Y12" s="106"/>
-      <c r="Z12" s="106"/>
-      <c r="AA12" s="106"/>
-      <c r="AB12" s="106"/>
-      <c r="AC12" s="106"/>
-      <c r="AD12" s="106"/>
-      <c r="AE12" s="106"/>
-      <c r="AF12" s="106"/>
-      <c r="AG12" s="106"/>
-      <c r="AH12" s="106"/>
-      <c r="AI12" s="106"/>
-      <c r="AJ12" s="106"/>
-      <c r="AK12" s="106"/>
-      <c r="AL12" s="106"/>
-      <c r="AM12" s="106"/>
-      <c r="AN12" s="106"/>
-      <c r="AO12" s="106"/>
-      <c r="AP12" s="106"/>
-      <c r="AQ12" s="106"/>
-      <c r="AR12" s="106"/>
-      <c r="AS12" s="106"/>
-      <c r="AT12" s="106"/>
-      <c r="AU12" s="106"/>
-      <c r="AV12" s="106"/>
-      <c r="AW12" s="106"/>
-      <c r="AX12" s="106"/>
-      <c r="AY12" s="106"/>
-      <c r="AZ12" s="106"/>
-      <c r="BA12" s="106"/>
-      <c r="BB12" s="106"/>
-      <c r="BC12" s="106"/>
-      <c r="BD12" s="106"/>
-      <c r="BE12" s="106"/>
-      <c r="BF12" s="106"/>
-      <c r="BG12" s="106"/>
-      <c r="BH12" s="106"/>
-      <c r="BI12" s="106"/>
-      <c r="BJ12" s="106"/>
-      <c r="BK12" s="106"/>
-      <c r="BL12" s="106"/>
-      <c r="BM12" s="106"/>
-      <c r="BN12" s="106"/>
+      <c r="B12" s="53" t="s">
+        <v>153</v>
+      </c>
+      <c r="D12" s="55"/>
+      <c r="E12" s="101">
+        <v>45201</v>
+      </c>
+      <c r="F12" s="101">
+        <f>IF(ISBLANK(E12)," - ",IF(G12=0,E12,E12+G12-1))</f>
+        <v>45205</v>
+      </c>
+      <c r="G12" s="56">
+        <v>5</v>
+      </c>
+      <c r="H12" s="57"/>
+      <c r="I12" s="58">
+        <f>IF(OR(F12=0,E12=0)," - ",NETWORKDAYS(E12,F12))</f>
+        <v>5</v>
+      </c>
+      <c r="J12" s="95"/>
+      <c r="K12" s="108"/>
+      <c r="L12" s="108"/>
+      <c r="M12" s="108"/>
+      <c r="N12" s="108"/>
+      <c r="O12" s="108"/>
+      <c r="P12" s="108"/>
+      <c r="Q12" s="108"/>
+      <c r="R12" s="108"/>
+      <c r="S12" s="108"/>
+      <c r="T12" s="108"/>
+      <c r="U12" s="108"/>
+      <c r="V12" s="108"/>
+      <c r="W12" s="108"/>
+      <c r="X12" s="108"/>
+      <c r="Y12" s="108"/>
+      <c r="Z12" s="108"/>
+      <c r="AA12" s="108"/>
+      <c r="AB12" s="108"/>
+      <c r="AC12" s="108"/>
+      <c r="AD12" s="108"/>
+      <c r="AE12" s="108"/>
+      <c r="AF12" s="108"/>
+      <c r="AG12" s="108"/>
+      <c r="AH12" s="108"/>
+      <c r="AI12" s="108"/>
+      <c r="AJ12" s="108"/>
+      <c r="AK12" s="108"/>
+      <c r="AL12" s="108"/>
+      <c r="AM12" s="108"/>
+      <c r="AN12" s="108"/>
+      <c r="AO12" s="108"/>
+      <c r="AP12" s="108"/>
+      <c r="AQ12" s="108"/>
+      <c r="AR12" s="108"/>
+      <c r="AS12" s="108"/>
+      <c r="AT12" s="108"/>
+      <c r="AU12" s="108"/>
+      <c r="AV12" s="108"/>
+      <c r="AW12" s="108"/>
+      <c r="AX12" s="108"/>
+      <c r="AY12" s="108"/>
+      <c r="AZ12" s="108"/>
+      <c r="BA12" s="108"/>
+      <c r="BB12" s="108"/>
+      <c r="BC12" s="108"/>
+      <c r="BD12" s="108"/>
+      <c r="BE12" s="108"/>
+      <c r="BF12" s="108"/>
+      <c r="BG12" s="108"/>
+      <c r="BH12" s="108"/>
+      <c r="BI12" s="108"/>
+      <c r="BJ12" s="108"/>
+      <c r="BK12" s="108"/>
+      <c r="BL12" s="108"/>
+      <c r="BM12" s="108"/>
+      <c r="BN12" s="108"/>
     </row>
     <row r="13" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
-        <v>1.4.1</v>
-      </c>
-      <c r="B13" s="127" t="s">
-        <v>137</v>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>2.1</v>
+      </c>
+      <c r="B13" s="125" t="s">
+        <v>146</v>
+      </c>
+      <c r="C13" s="60" t="s">
+        <v>147</v>
       </c>
       <c r="D13" s="126"/>
       <c r="E13" s="99">
-        <v>43133</v>
+        <f>E12</f>
+        <v>45201</v>
       </c>
       <c r="F13" s="100">
         <f t="shared" si="6"/>
-        <v>43134</v>
+        <v>45203</v>
       </c>
       <c r="G13" s="61">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H13" s="62">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I13" s="63">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J13" s="94"/>
       <c r="K13" s="106"/>
@@ -5030,29 +5148,33 @@
     </row>
     <row r="14" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
-        <v>1.4.2</v>
-      </c>
-      <c r="B14" s="127" t="s">
-        <v>137</v>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>2.2</v>
+      </c>
+      <c r="B14" s="125" t="s">
+        <v>149</v>
+      </c>
+      <c r="C14" s="60" t="s">
+        <v>142</v>
       </c>
       <c r="D14" s="126"/>
       <c r="E14" s="99">
-        <v>43135</v>
+        <f>E12</f>
+        <v>45201</v>
       </c>
       <c r="F14" s="100">
-        <f t="shared" si="6"/>
-        <v>43137</v>
+        <f t="shared" ref="F14" si="7">IF(ISBLANK(E14)," - ",IF(G14=0,E14,E14+G14-1))</f>
+        <v>45205</v>
       </c>
       <c r="G14" s="61">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H14" s="62">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I14" s="63">
-        <f t="shared" si="4"/>
-        <v>2</v>
+        <f t="shared" ref="I14" si="8">IF(OR(F14=0,E14=0)," - ",NETWORKDAYS(E14,F14))</f>
+        <v>5</v>
       </c>
       <c r="J14" s="94"/>
       <c r="K14" s="106"/>
@@ -5114,25 +5236,29 @@
     </row>
     <row r="15" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="59" t="str">
-        <f t="shared" si="5"/>
-        <v>1.5</v>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>2.3</v>
       </c>
       <c r="B15" s="125" t="s">
-        <v>11</v>
+        <v>151</v>
+      </c>
+      <c r="C15" s="60" t="s">
+        <v>152</v>
       </c>
       <c r="D15" s="126"/>
       <c r="E15" s="99">
-        <v>43136</v>
+        <f>E12</f>
+        <v>45201</v>
       </c>
       <c r="F15" s="100">
         <f t="shared" si="6"/>
-        <v>43140</v>
+        <v>45205</v>
       </c>
       <c r="G15" s="61">
         <v>5</v>
       </c>
       <c r="H15" s="62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15" s="63">
         <f t="shared" si="4"/>
@@ -5196,115 +5322,117 @@
       <c r="BM15" s="106"/>
       <c r="BN15" s="106"/>
     </row>
-    <row r="16" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A16" s="59" t="str">
-        <f t="shared" si="5"/>
-        <v>1.6</v>
-      </c>
-      <c r="B16" s="125" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="126"/>
-      <c r="E16" s="99">
-        <v>43134</v>
-      </c>
-      <c r="F16" s="100">
+    <row r="16" spans="1:66" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A16" s="52" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>3</v>
+      </c>
+      <c r="B16" s="53" t="s">
+        <v>156</v>
+      </c>
+      <c r="D16" s="55"/>
+      <c r="E16" s="101">
+        <v>45208</v>
+      </c>
+      <c r="F16" s="101">
         <f t="shared" si="6"/>
-        <v>43140</v>
-      </c>
-      <c r="G16" s="61">
-        <v>7</v>
-      </c>
-      <c r="H16" s="62">
-        <v>0</v>
-      </c>
-      <c r="I16" s="63">
+        <v>45212</v>
+      </c>
+      <c r="G16" s="56">
+        <v>5</v>
+      </c>
+      <c r="H16" s="57"/>
+      <c r="I16" s="58">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="J16" s="94"/>
-      <c r="K16" s="106"/>
-      <c r="L16" s="106"/>
-      <c r="M16" s="106"/>
-      <c r="N16" s="106"/>
-      <c r="O16" s="106"/>
-      <c r="P16" s="106"/>
-      <c r="Q16" s="106"/>
-      <c r="R16" s="106"/>
-      <c r="S16" s="106"/>
-      <c r="T16" s="106"/>
-      <c r="U16" s="106"/>
-      <c r="V16" s="106"/>
-      <c r="W16" s="106"/>
-      <c r="X16" s="106"/>
-      <c r="Y16" s="106"/>
-      <c r="Z16" s="106"/>
-      <c r="AA16" s="106"/>
-      <c r="AB16" s="106"/>
-      <c r="AC16" s="106"/>
-      <c r="AD16" s="106"/>
-      <c r="AE16" s="106"/>
-      <c r="AF16" s="106"/>
-      <c r="AG16" s="106"/>
-      <c r="AH16" s="106"/>
-      <c r="AI16" s="106"/>
-      <c r="AJ16" s="106"/>
-      <c r="AK16" s="106"/>
-      <c r="AL16" s="106"/>
-      <c r="AM16" s="106"/>
-      <c r="AN16" s="106"/>
-      <c r="AO16" s="106"/>
-      <c r="AP16" s="106"/>
-      <c r="AQ16" s="106"/>
-      <c r="AR16" s="106"/>
-      <c r="AS16" s="106"/>
-      <c r="AT16" s="106"/>
-      <c r="AU16" s="106"/>
-      <c r="AV16" s="106"/>
-      <c r="AW16" s="106"/>
-      <c r="AX16" s="106"/>
-      <c r="AY16" s="106"/>
-      <c r="AZ16" s="106"/>
-      <c r="BA16" s="106"/>
-      <c r="BB16" s="106"/>
-      <c r="BC16" s="106"/>
-      <c r="BD16" s="106"/>
-      <c r="BE16" s="106"/>
-      <c r="BF16" s="106"/>
-      <c r="BG16" s="106"/>
-      <c r="BH16" s="106"/>
-      <c r="BI16" s="106"/>
-      <c r="BJ16" s="106"/>
-      <c r="BK16" s="106"/>
-      <c r="BL16" s="106"/>
-      <c r="BM16" s="106"/>
-      <c r="BN16" s="106"/>
+      <c r="J16" s="95"/>
+      <c r="K16" s="108"/>
+      <c r="L16" s="108"/>
+      <c r="M16" s="108"/>
+      <c r="N16" s="108"/>
+      <c r="O16" s="108"/>
+      <c r="P16" s="108"/>
+      <c r="Q16" s="108"/>
+      <c r="R16" s="108"/>
+      <c r="S16" s="108"/>
+      <c r="T16" s="108"/>
+      <c r="U16" s="108"/>
+      <c r="V16" s="108"/>
+      <c r="W16" s="108"/>
+      <c r="X16" s="108"/>
+      <c r="Y16" s="108"/>
+      <c r="Z16" s="108"/>
+      <c r="AA16" s="108"/>
+      <c r="AB16" s="108"/>
+      <c r="AC16" s="108"/>
+      <c r="AD16" s="108"/>
+      <c r="AE16" s="108"/>
+      <c r="AF16" s="108"/>
+      <c r="AG16" s="108"/>
+      <c r="AH16" s="108"/>
+      <c r="AI16" s="108"/>
+      <c r="AJ16" s="108"/>
+      <c r="AK16" s="108"/>
+      <c r="AL16" s="108"/>
+      <c r="AM16" s="108"/>
+      <c r="AN16" s="108"/>
+      <c r="AO16" s="108"/>
+      <c r="AP16" s="108"/>
+      <c r="AQ16" s="108"/>
+      <c r="AR16" s="108"/>
+      <c r="AS16" s="108"/>
+      <c r="AT16" s="108"/>
+      <c r="AU16" s="108"/>
+      <c r="AV16" s="108"/>
+      <c r="AW16" s="108"/>
+      <c r="AX16" s="108"/>
+      <c r="AY16" s="108"/>
+      <c r="AZ16" s="108"/>
+      <c r="BA16" s="108"/>
+      <c r="BB16" s="108"/>
+      <c r="BC16" s="108"/>
+      <c r="BD16" s="108"/>
+      <c r="BE16" s="108"/>
+      <c r="BF16" s="108"/>
+      <c r="BG16" s="108"/>
+      <c r="BH16" s="108"/>
+      <c r="BI16" s="108"/>
+      <c r="BJ16" s="108"/>
+      <c r="BK16" s="108"/>
+      <c r="BL16" s="108"/>
+      <c r="BM16" s="108"/>
+      <c r="BN16" s="108"/>
     </row>
     <row r="17" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="59" t="str">
-        <f t="shared" si="5"/>
-        <v>1.7</v>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>3.1</v>
       </c>
       <c r="B17" s="125" t="s">
-        <v>11</v>
+        <v>150</v>
+      </c>
+      <c r="C17" s="60" t="s">
+        <v>145</v>
       </c>
       <c r="D17" s="126"/>
       <c r="E17" s="99">
-        <v>43141</v>
+        <f>E16</f>
+        <v>45208</v>
       </c>
       <c r="F17" s="100">
         <f t="shared" si="6"/>
-        <v>43147</v>
+        <v>45211</v>
       </c>
       <c r="G17" s="61">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H17" s="62">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I17" s="63">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J17" s="94"/>
       <c r="K17" s="106"/>
@@ -5364,109 +5492,123 @@
       <c r="BM17" s="106"/>
       <c r="BN17" s="106"/>
     </row>
-    <row r="18" spans="1:66" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A18" s="52" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>2</v>
-      </c>
-      <c r="B18" s="53" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="55"/>
-      <c r="E18" s="101"/>
-      <c r="F18" s="101" t="str">
+    <row r="18" spans="1:66" s="60" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A18" s="59" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>3.2</v>
+      </c>
+      <c r="B18" s="125" t="s">
+        <v>154</v>
+      </c>
+      <c r="C18" s="60" t="s">
+        <v>152</v>
+      </c>
+      <c r="D18" s="126"/>
+      <c r="E18" s="99">
+        <f>E16</f>
+        <v>45208</v>
+      </c>
+      <c r="F18" s="100">
         <f t="shared" si="6"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G18" s="56"/>
-      <c r="H18" s="57"/>
-      <c r="I18" s="58" t="str">
+        <v>45210</v>
+      </c>
+      <c r="G18" s="61">
+        <v>3</v>
+      </c>
+      <c r="H18" s="62">
+        <v>0</v>
+      </c>
+      <c r="I18" s="63">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J18" s="95"/>
-      <c r="K18" s="108"/>
-      <c r="L18" s="108"/>
-      <c r="M18" s="108"/>
-      <c r="N18" s="108"/>
-      <c r="O18" s="108"/>
-      <c r="P18" s="108"/>
-      <c r="Q18" s="108"/>
-      <c r="R18" s="108"/>
-      <c r="S18" s="108"/>
-      <c r="T18" s="108"/>
-      <c r="U18" s="108"/>
-      <c r="V18" s="108"/>
-      <c r="W18" s="108"/>
-      <c r="X18" s="108"/>
-      <c r="Y18" s="108"/>
-      <c r="Z18" s="108"/>
-      <c r="AA18" s="108"/>
-      <c r="AB18" s="108"/>
-      <c r="AC18" s="108"/>
-      <c r="AD18" s="108"/>
-      <c r="AE18" s="108"/>
-      <c r="AF18" s="108"/>
-      <c r="AG18" s="108"/>
-      <c r="AH18" s="108"/>
-      <c r="AI18" s="108"/>
-      <c r="AJ18" s="108"/>
-      <c r="AK18" s="108"/>
-      <c r="AL18" s="108"/>
-      <c r="AM18" s="108"/>
-      <c r="AN18" s="108"/>
-      <c r="AO18" s="108"/>
-      <c r="AP18" s="108"/>
-      <c r="AQ18" s="108"/>
-      <c r="AR18" s="108"/>
-      <c r="AS18" s="108"/>
-      <c r="AT18" s="108"/>
-      <c r="AU18" s="108"/>
-      <c r="AV18" s="108"/>
-      <c r="AW18" s="108"/>
-      <c r="AX18" s="108"/>
-      <c r="AY18" s="108"/>
-      <c r="AZ18" s="108"/>
-      <c r="BA18" s="108"/>
-      <c r="BB18" s="108"/>
-      <c r="BC18" s="108"/>
-      <c r="BD18" s="108"/>
-      <c r="BE18" s="108"/>
-      <c r="BF18" s="108"/>
-      <c r="BG18" s="108"/>
-      <c r="BH18" s="108"/>
-      <c r="BI18" s="108"/>
-      <c r="BJ18" s="108"/>
-      <c r="BK18" s="108"/>
-      <c r="BL18" s="108"/>
-      <c r="BM18" s="108"/>
-      <c r="BN18" s="108"/>
+        <v>3</v>
+      </c>
+      <c r="J18" s="94"/>
+      <c r="K18" s="106"/>
+      <c r="L18" s="106"/>
+      <c r="M18" s="106"/>
+      <c r="N18" s="106"/>
+      <c r="O18" s="106"/>
+      <c r="P18" s="106"/>
+      <c r="Q18" s="106"/>
+      <c r="R18" s="106"/>
+      <c r="S18" s="106"/>
+      <c r="T18" s="106"/>
+      <c r="U18" s="106"/>
+      <c r="V18" s="106"/>
+      <c r="W18" s="106"/>
+      <c r="X18" s="106"/>
+      <c r="Y18" s="106"/>
+      <c r="Z18" s="106"/>
+      <c r="AA18" s="106"/>
+      <c r="AB18" s="106"/>
+      <c r="AC18" s="106"/>
+      <c r="AD18" s="106"/>
+      <c r="AE18" s="106"/>
+      <c r="AF18" s="106"/>
+      <c r="AG18" s="106"/>
+      <c r="AH18" s="106"/>
+      <c r="AI18" s="106"/>
+      <c r="AJ18" s="106"/>
+      <c r="AK18" s="106"/>
+      <c r="AL18" s="106"/>
+      <c r="AM18" s="106"/>
+      <c r="AN18" s="106"/>
+      <c r="AO18" s="106"/>
+      <c r="AP18" s="106"/>
+      <c r="AQ18" s="106"/>
+      <c r="AR18" s="106"/>
+      <c r="AS18" s="106"/>
+      <c r="AT18" s="106"/>
+      <c r="AU18" s="106"/>
+      <c r="AV18" s="106"/>
+      <c r="AW18" s="106"/>
+      <c r="AX18" s="106"/>
+      <c r="AY18" s="106"/>
+      <c r="AZ18" s="106"/>
+      <c r="BA18" s="106"/>
+      <c r="BB18" s="106"/>
+      <c r="BC18" s="106"/>
+      <c r="BD18" s="106"/>
+      <c r="BE18" s="106"/>
+      <c r="BF18" s="106"/>
+      <c r="BG18" s="106"/>
+      <c r="BH18" s="106"/>
+      <c r="BI18" s="106"/>
+      <c r="BJ18" s="106"/>
+      <c r="BK18" s="106"/>
+      <c r="BL18" s="106"/>
+      <c r="BM18" s="106"/>
+      <c r="BN18" s="106"/>
     </row>
     <row r="19" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>2.1</v>
+        <v>3.3</v>
       </c>
       <c r="B19" s="125" t="s">
-        <v>11</v>
+        <v>155</v>
+      </c>
+      <c r="C19" s="60" t="s">
+        <v>142</v>
       </c>
       <c r="D19" s="126"/>
       <c r="E19" s="99">
-        <v>43141</v>
+        <f>E16</f>
+        <v>45208</v>
       </c>
       <c r="F19" s="100">
         <f t="shared" si="6"/>
-        <v>43144</v>
+        <v>45208</v>
       </c>
       <c r="G19" s="61">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H19" s="62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" s="63">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J19" s="94"/>
       <c r="K19" s="106"/>
@@ -5526,31 +5668,35 @@
       <c r="BM19" s="106"/>
       <c r="BN19" s="106"/>
     </row>
-    <row r="20" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:66" s="60" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A20" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>2.2</v>
+        <v>3.4</v>
       </c>
       <c r="B20" s="125" t="s">
-        <v>11</v>
+        <v>161</v>
+      </c>
+      <c r="C20" s="60" t="s">
+        <v>142</v>
       </c>
       <c r="D20" s="126"/>
       <c r="E20" s="99">
-        <v>43145</v>
+        <f>E16+1</f>
+        <v>45209</v>
       </c>
       <c r="F20" s="100">
         <f t="shared" si="6"/>
-        <v>43147</v>
+        <v>45209</v>
       </c>
       <c r="G20" s="61">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H20" s="62">
         <v>0</v>
       </c>
       <c r="I20" s="63">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J20" s="94"/>
       <c r="K20" s="106"/>
@@ -5610,31 +5756,35 @@
       <c r="BM20" s="106"/>
       <c r="BN20" s="106"/>
     </row>
-    <row r="21" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:66" s="60" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A21" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>2.3</v>
+        <v>3.5</v>
       </c>
       <c r="B21" s="125" t="s">
-        <v>11</v>
+        <v>157</v>
+      </c>
+      <c r="C21" s="60" t="s">
+        <v>158</v>
       </c>
       <c r="D21" s="126"/>
       <c r="E21" s="99">
-        <v>43145</v>
+        <f>F20+1</f>
+        <v>45210</v>
       </c>
       <c r="F21" s="100">
         <f t="shared" si="6"/>
-        <v>43147</v>
+        <v>45210</v>
       </c>
       <c r="G21" s="61">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H21" s="62">
         <v>0</v>
       </c>
       <c r="I21" s="63">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J21" s="94"/>
       <c r="K21" s="106"/>
@@ -5697,30 +5847,34 @@
     <row r="22" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>2.4</v>
+        <v>3.6</v>
       </c>
       <c r="B22" s="125" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="126"/>
-      <c r="E22" s="99">
-        <v>43148</v>
-      </c>
-      <c r="F22" s="100">
+        <v>159</v>
+      </c>
+      <c r="C22" s="60" t="s">
+        <v>160</v>
+      </c>
+      <c r="D22" s="172"/>
+      <c r="E22" s="173">
+        <f>F20+1</f>
+        <v>45210</v>
+      </c>
+      <c r="F22" s="174">
         <f t="shared" si="6"/>
-        <v>43153</v>
-      </c>
-      <c r="G22" s="61">
-        <v>6</v>
-      </c>
-      <c r="H22" s="62">
+        <v>45210</v>
+      </c>
+      <c r="G22" s="175">
+        <v>1</v>
+      </c>
+      <c r="H22" s="176">
         <v>0</v>
       </c>
-      <c r="I22" s="63">
+      <c r="I22" s="177">
         <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="J22" s="94"/>
+        <v>1</v>
+      </c>
+      <c r="J22" s="178"/>
       <c r="K22" s="106"/>
       <c r="L22" s="106"/>
       <c r="M22" s="106"/>
@@ -5778,193 +5932,193 @@
       <c r="BM22" s="106"/>
       <c r="BN22" s="106"/>
     </row>
-    <row r="23" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A23" s="59" t="str">
+    <row r="23" spans="1:66" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A23" s="52" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>4</v>
+      </c>
+      <c r="B23" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="55"/>
+      <c r="E23" s="101"/>
+      <c r="F23" s="101" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G23" s="56"/>
+      <c r="H23" s="57"/>
+      <c r="I23" s="58" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J23" s="95"/>
+      <c r="K23" s="108"/>
+      <c r="L23" s="108"/>
+      <c r="M23" s="108"/>
+      <c r="N23" s="108"/>
+      <c r="O23" s="108"/>
+      <c r="P23" s="108"/>
+      <c r="Q23" s="108"/>
+      <c r="R23" s="108"/>
+      <c r="S23" s="108"/>
+      <c r="T23" s="108"/>
+      <c r="U23" s="108"/>
+      <c r="V23" s="108"/>
+      <c r="W23" s="108"/>
+      <c r="X23" s="108"/>
+      <c r="Y23" s="108"/>
+      <c r="Z23" s="108"/>
+      <c r="AA23" s="108"/>
+      <c r="AB23" s="108"/>
+      <c r="AC23" s="108"/>
+      <c r="AD23" s="108"/>
+      <c r="AE23" s="108"/>
+      <c r="AF23" s="108"/>
+      <c r="AG23" s="108"/>
+      <c r="AH23" s="108"/>
+      <c r="AI23" s="108"/>
+      <c r="AJ23" s="108"/>
+      <c r="AK23" s="108"/>
+      <c r="AL23" s="108"/>
+      <c r="AM23" s="108"/>
+      <c r="AN23" s="108"/>
+      <c r="AO23" s="108"/>
+      <c r="AP23" s="108"/>
+      <c r="AQ23" s="108"/>
+      <c r="AR23" s="108"/>
+      <c r="AS23" s="108"/>
+      <c r="AT23" s="108"/>
+      <c r="AU23" s="108"/>
+      <c r="AV23" s="108"/>
+      <c r="AW23" s="108"/>
+      <c r="AX23" s="108"/>
+      <c r="AY23" s="108"/>
+      <c r="AZ23" s="108"/>
+      <c r="BA23" s="108"/>
+      <c r="BB23" s="108"/>
+      <c r="BC23" s="108"/>
+      <c r="BD23" s="108"/>
+      <c r="BE23" s="108"/>
+      <c r="BF23" s="108"/>
+      <c r="BG23" s="108"/>
+      <c r="BH23" s="108"/>
+      <c r="BI23" s="108"/>
+      <c r="BJ23" s="108"/>
+      <c r="BK23" s="108"/>
+      <c r="BL23" s="108"/>
+      <c r="BM23" s="108"/>
+      <c r="BN23" s="108"/>
+    </row>
+    <row r="24" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A24" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>2.5</v>
-      </c>
-      <c r="B23" s="125" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="126"/>
-      <c r="E23" s="99">
-        <v>43154</v>
-      </c>
-      <c r="F23" s="100">
+        <v>4.1</v>
+      </c>
+      <c r="B24" s="125" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="126"/>
+      <c r="E24" s="99">
+        <v>43129</v>
+      </c>
+      <c r="F24" s="100">
         <f t="shared" si="6"/>
-        <v>43156</v>
-      </c>
-      <c r="G23" s="61">
-        <v>3</v>
-      </c>
-      <c r="H23" s="62">
+        <v>43129</v>
+      </c>
+      <c r="G24" s="61">
+        <v>1</v>
+      </c>
+      <c r="H24" s="62">
         <v>0</v>
       </c>
-      <c r="I23" s="63">
+      <c r="I24" s="63">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="J23" s="94"/>
-      <c r="K23" s="106"/>
-      <c r="L23" s="106"/>
-      <c r="M23" s="106"/>
-      <c r="N23" s="106"/>
-      <c r="O23" s="106"/>
-      <c r="P23" s="106"/>
-      <c r="Q23" s="106"/>
-      <c r="R23" s="106"/>
-      <c r="S23" s="106"/>
-      <c r="T23" s="106"/>
-      <c r="U23" s="106"/>
-      <c r="V23" s="106"/>
-      <c r="W23" s="106"/>
-      <c r="X23" s="106"/>
-      <c r="Y23" s="106"/>
-      <c r="Z23" s="106"/>
-      <c r="AA23" s="106"/>
-      <c r="AB23" s="106"/>
-      <c r="AC23" s="106"/>
-      <c r="AD23" s="106"/>
-      <c r="AE23" s="106"/>
-      <c r="AF23" s="106"/>
-      <c r="AG23" s="106"/>
-      <c r="AH23" s="106"/>
-      <c r="AI23" s="106"/>
-      <c r="AJ23" s="106"/>
-      <c r="AK23" s="106"/>
-      <c r="AL23" s="106"/>
-      <c r="AM23" s="106"/>
-      <c r="AN23" s="106"/>
-      <c r="AO23" s="106"/>
-      <c r="AP23" s="106"/>
-      <c r="AQ23" s="106"/>
-      <c r="AR23" s="106"/>
-      <c r="AS23" s="106"/>
-      <c r="AT23" s="106"/>
-      <c r="AU23" s="106"/>
-      <c r="AV23" s="106"/>
-      <c r="AW23" s="106"/>
-      <c r="AX23" s="106"/>
-      <c r="AY23" s="106"/>
-      <c r="AZ23" s="106"/>
-      <c r="BA23" s="106"/>
-      <c r="BB23" s="106"/>
-      <c r="BC23" s="106"/>
-      <c r="BD23" s="106"/>
-      <c r="BE23" s="106"/>
-      <c r="BF23" s="106"/>
-      <c r="BG23" s="106"/>
-      <c r="BH23" s="106"/>
-      <c r="BI23" s="106"/>
-      <c r="BJ23" s="106"/>
-      <c r="BK23" s="106"/>
-      <c r="BL23" s="106"/>
-      <c r="BM23" s="106"/>
-      <c r="BN23" s="106"/>
-    </row>
-    <row r="24" spans="1:66" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A24" s="52" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>3</v>
-      </c>
-      <c r="B24" s="53" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="55"/>
-      <c r="E24" s="101"/>
-      <c r="F24" s="101" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G24" s="56"/>
-      <c r="H24" s="57"/>
-      <c r="I24" s="58" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J24" s="95"/>
-      <c r="K24" s="108"/>
-      <c r="L24" s="108"/>
-      <c r="M24" s="108"/>
-      <c r="N24" s="108"/>
-      <c r="O24" s="108"/>
-      <c r="P24" s="108"/>
-      <c r="Q24" s="108"/>
-      <c r="R24" s="108"/>
-      <c r="S24" s="108"/>
-      <c r="T24" s="108"/>
-      <c r="U24" s="108"/>
-      <c r="V24" s="108"/>
-      <c r="W24" s="108"/>
-      <c r="X24" s="108"/>
-      <c r="Y24" s="108"/>
-      <c r="Z24" s="108"/>
-      <c r="AA24" s="108"/>
-      <c r="AB24" s="108"/>
-      <c r="AC24" s="108"/>
-      <c r="AD24" s="108"/>
-      <c r="AE24" s="108"/>
-      <c r="AF24" s="108"/>
-      <c r="AG24" s="108"/>
-      <c r="AH24" s="108"/>
-      <c r="AI24" s="108"/>
-      <c r="AJ24" s="108"/>
-      <c r="AK24" s="108"/>
-      <c r="AL24" s="108"/>
-      <c r="AM24" s="108"/>
-      <c r="AN24" s="108"/>
-      <c r="AO24" s="108"/>
-      <c r="AP24" s="108"/>
-      <c r="AQ24" s="108"/>
-      <c r="AR24" s="108"/>
-      <c r="AS24" s="108"/>
-      <c r="AT24" s="108"/>
-      <c r="AU24" s="108"/>
-      <c r="AV24" s="108"/>
-      <c r="AW24" s="108"/>
-      <c r="AX24" s="108"/>
-      <c r="AY24" s="108"/>
-      <c r="AZ24" s="108"/>
-      <c r="BA24" s="108"/>
-      <c r="BB24" s="108"/>
-      <c r="BC24" s="108"/>
-      <c r="BD24" s="108"/>
-      <c r="BE24" s="108"/>
-      <c r="BF24" s="108"/>
-      <c r="BG24" s="108"/>
-      <c r="BH24" s="108"/>
-      <c r="BI24" s="108"/>
-      <c r="BJ24" s="108"/>
-      <c r="BK24" s="108"/>
-      <c r="BL24" s="108"/>
-      <c r="BM24" s="108"/>
-      <c r="BN24" s="108"/>
+      <c r="J24" s="94"/>
+      <c r="K24" s="106"/>
+      <c r="L24" s="106"/>
+      <c r="M24" s="106"/>
+      <c r="N24" s="106"/>
+      <c r="O24" s="106"/>
+      <c r="P24" s="106"/>
+      <c r="Q24" s="106"/>
+      <c r="R24" s="106"/>
+      <c r="S24" s="106"/>
+      <c r="T24" s="106"/>
+      <c r="U24" s="106"/>
+      <c r="V24" s="106"/>
+      <c r="W24" s="106"/>
+      <c r="X24" s="106"/>
+      <c r="Y24" s="106"/>
+      <c r="Z24" s="106"/>
+      <c r="AA24" s="106"/>
+      <c r="AB24" s="106"/>
+      <c r="AC24" s="106"/>
+      <c r="AD24" s="106"/>
+      <c r="AE24" s="106"/>
+      <c r="AF24" s="106"/>
+      <c r="AG24" s="106"/>
+      <c r="AH24" s="106"/>
+      <c r="AI24" s="106"/>
+      <c r="AJ24" s="106"/>
+      <c r="AK24" s="106"/>
+      <c r="AL24" s="106"/>
+      <c r="AM24" s="106"/>
+      <c r="AN24" s="106"/>
+      <c r="AO24" s="106"/>
+      <c r="AP24" s="106"/>
+      <c r="AQ24" s="106"/>
+      <c r="AR24" s="106"/>
+      <c r="AS24" s="106"/>
+      <c r="AT24" s="106"/>
+      <c r="AU24" s="106"/>
+      <c r="AV24" s="106"/>
+      <c r="AW24" s="106"/>
+      <c r="AX24" s="106"/>
+      <c r="AY24" s="106"/>
+      <c r="AZ24" s="106"/>
+      <c r="BA24" s="106"/>
+      <c r="BB24" s="106"/>
+      <c r="BC24" s="106"/>
+      <c r="BD24" s="106"/>
+      <c r="BE24" s="106"/>
+      <c r="BF24" s="106"/>
+      <c r="BG24" s="106"/>
+      <c r="BH24" s="106"/>
+      <c r="BI24" s="106"/>
+      <c r="BJ24" s="106"/>
+      <c r="BK24" s="106"/>
+      <c r="BL24" s="106"/>
+      <c r="BM24" s="106"/>
+      <c r="BN24" s="106"/>
     </row>
     <row r="25" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>3.1</v>
+        <v>4.2</v>
       </c>
       <c r="B25" s="125" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D25" s="126"/>
       <c r="E25" s="99">
-        <v>43141</v>
+        <v>43130</v>
       </c>
       <c r="F25" s="100">
         <f t="shared" si="6"/>
-        <v>43144</v>
+        <v>43130</v>
       </c>
       <c r="G25" s="61">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H25" s="62">
         <v>0</v>
       </c>
       <c r="I25" s="63">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J25" s="94"/>
       <c r="K25" s="106"/>
@@ -6027,28 +6181,28 @@
     <row r="26" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>3.2</v>
+        <v>4.3</v>
       </c>
       <c r="B26" s="125" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D26" s="126"/>
       <c r="E26" s="99">
-        <v>43145</v>
+        <v>43131</v>
       </c>
       <c r="F26" s="100">
         <f t="shared" si="6"/>
-        <v>43147</v>
+        <v>43131</v>
       </c>
       <c r="G26" s="61">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H26" s="62">
         <v>0</v>
       </c>
       <c r="I26" s="63">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J26" s="94"/>
       <c r="K26" s="106"/>
@@ -6111,28 +6265,28 @@
     <row r="27" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>3.3</v>
+        <v>4.4</v>
       </c>
       <c r="B27" s="125" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D27" s="126"/>
       <c r="E27" s="99">
-        <v>43145</v>
+        <v>43132</v>
       </c>
       <c r="F27" s="100">
         <f t="shared" si="6"/>
-        <v>43147</v>
+        <v>43132</v>
       </c>
       <c r="G27" s="61">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H27" s="62">
         <v>0</v>
       </c>
       <c r="I27" s="63">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J27" s="94"/>
       <c r="K27" s="106"/>
@@ -6195,28 +6349,28 @@
     <row r="28" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>3.4</v>
+        <v>4.5</v>
       </c>
       <c r="B28" s="125" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D28" s="126"/>
       <c r="E28" s="99">
-        <v>43148</v>
+        <v>43133</v>
       </c>
       <c r="F28" s="100">
         <f t="shared" si="6"/>
-        <v>43153</v>
+        <v>43133</v>
       </c>
       <c r="G28" s="61">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H28" s="62">
         <v>0</v>
       </c>
       <c r="I28" s="63">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J28" s="94"/>
       <c r="K28" s="106"/>
@@ -6276,33 +6430,20 @@
       <c r="BM28" s="106"/>
       <c r="BN28" s="106"/>
     </row>
-    <row r="29" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A29" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>3.5</v>
-      </c>
-      <c r="B29" s="125" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" s="126"/>
-      <c r="E29" s="99">
-        <v>43154</v>
-      </c>
-      <c r="F29" s="100">
-        <f t="shared" si="6"/>
-        <v>43156</v>
-      </c>
-      <c r="G29" s="61">
-        <v>3</v>
-      </c>
-      <c r="H29" s="62">
-        <v>0</v>
-      </c>
-      <c r="I29" s="63">
+    <row r="29" spans="1:66" s="69" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A29" s="59"/>
+      <c r="B29" s="64"/>
+      <c r="C29" s="64"/>
+      <c r="D29" s="65"/>
+      <c r="E29" s="102"/>
+      <c r="F29" s="102"/>
+      <c r="G29" s="66"/>
+      <c r="H29" s="67"/>
+      <c r="I29" s="68" t="str">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J29" s="94"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J29" s="96"/>
       <c r="K29" s="106"/>
       <c r="L29" s="106"/>
       <c r="M29" s="106"/>
@@ -6360,111 +6501,90 @@
       <c r="BM29" s="106"/>
       <c r="BN29" s="106"/>
     </row>
-    <row r="30" spans="1:66" s="54" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A30" s="52" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>4</v>
-      </c>
-      <c r="B30" s="53" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" s="55"/>
-      <c r="E30" s="101"/>
-      <c r="F30" s="101" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G30" s="56"/>
-      <c r="H30" s="57"/>
-      <c r="I30" s="58" t="str">
+    <row r="30" spans="1:66" s="69" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A30" s="59"/>
+      <c r="B30" s="64"/>
+      <c r="C30" s="64"/>
+      <c r="D30" s="65"/>
+      <c r="E30" s="102"/>
+      <c r="F30" s="102"/>
+      <c r="G30" s="66"/>
+      <c r="H30" s="67"/>
+      <c r="I30" s="68" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J30" s="95"/>
-      <c r="K30" s="108"/>
-      <c r="L30" s="108"/>
-      <c r="M30" s="108"/>
-      <c r="N30" s="108"/>
-      <c r="O30" s="108"/>
-      <c r="P30" s="108"/>
-      <c r="Q30" s="108"/>
-      <c r="R30" s="108"/>
-      <c r="S30" s="108"/>
-      <c r="T30" s="108"/>
-      <c r="U30" s="108"/>
-      <c r="V30" s="108"/>
-      <c r="W30" s="108"/>
-      <c r="X30" s="108"/>
-      <c r="Y30" s="108"/>
-      <c r="Z30" s="108"/>
-      <c r="AA30" s="108"/>
-      <c r="AB30" s="108"/>
-      <c r="AC30" s="108"/>
-      <c r="AD30" s="108"/>
-      <c r="AE30" s="108"/>
-      <c r="AF30" s="108"/>
-      <c r="AG30" s="108"/>
-      <c r="AH30" s="108"/>
-      <c r="AI30" s="108"/>
-      <c r="AJ30" s="108"/>
-      <c r="AK30" s="108"/>
-      <c r="AL30" s="108"/>
-      <c r="AM30" s="108"/>
-      <c r="AN30" s="108"/>
-      <c r="AO30" s="108"/>
-      <c r="AP30" s="108"/>
-      <c r="AQ30" s="108"/>
-      <c r="AR30" s="108"/>
-      <c r="AS30" s="108"/>
-      <c r="AT30" s="108"/>
-      <c r="AU30" s="108"/>
-      <c r="AV30" s="108"/>
-      <c r="AW30" s="108"/>
-      <c r="AX30" s="108"/>
-      <c r="AY30" s="108"/>
-      <c r="AZ30" s="108"/>
-      <c r="BA30" s="108"/>
-      <c r="BB30" s="108"/>
-      <c r="BC30" s="108"/>
-      <c r="BD30" s="108"/>
-      <c r="BE30" s="108"/>
-      <c r="BF30" s="108"/>
-      <c r="BG30" s="108"/>
-      <c r="BH30" s="108"/>
-      <c r="BI30" s="108"/>
-      <c r="BJ30" s="108"/>
-      <c r="BK30" s="108"/>
-      <c r="BL30" s="108"/>
-      <c r="BM30" s="108"/>
-      <c r="BN30" s="108"/>
-    </row>
-    <row r="31" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A31" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>4.1</v>
-      </c>
-      <c r="B31" s="125" t="s">
-        <v>11</v>
-      </c>
-      <c r="D31" s="126"/>
-      <c r="E31" s="99">
-        <v>43129</v>
-      </c>
-      <c r="F31" s="100">
-        <f t="shared" si="6"/>
-        <v>43129</v>
-      </c>
-      <c r="G31" s="61">
+      <c r="J30" s="96"/>
+      <c r="K30" s="106"/>
+      <c r="L30" s="106"/>
+      <c r="M30" s="106"/>
+      <c r="N30" s="106"/>
+      <c r="O30" s="106"/>
+      <c r="P30" s="106"/>
+      <c r="Q30" s="106"/>
+      <c r="R30" s="106"/>
+      <c r="S30" s="106"/>
+      <c r="T30" s="106"/>
+      <c r="U30" s="106"/>
+      <c r="V30" s="106"/>
+      <c r="W30" s="106"/>
+      <c r="X30" s="106"/>
+      <c r="Y30" s="106"/>
+      <c r="Z30" s="106"/>
+      <c r="AA30" s="106"/>
+      <c r="AB30" s="106"/>
+      <c r="AC30" s="106"/>
+      <c r="AD30" s="106"/>
+      <c r="AE30" s="106"/>
+      <c r="AF30" s="106"/>
+      <c r="AG30" s="106"/>
+      <c r="AH30" s="106"/>
+      <c r="AI30" s="106"/>
+      <c r="AJ30" s="106"/>
+      <c r="AK30" s="106"/>
+      <c r="AL30" s="106"/>
+      <c r="AM30" s="106"/>
+      <c r="AN30" s="106"/>
+      <c r="AO30" s="106"/>
+      <c r="AP30" s="106"/>
+      <c r="AQ30" s="106"/>
+      <c r="AR30" s="106"/>
+      <c r="AS30" s="106"/>
+      <c r="AT30" s="106"/>
+      <c r="AU30" s="106"/>
+      <c r="AV30" s="106"/>
+      <c r="AW30" s="106"/>
+      <c r="AX30" s="106"/>
+      <c r="AY30" s="106"/>
+      <c r="AZ30" s="106"/>
+      <c r="BA30" s="106"/>
+      <c r="BB30" s="106"/>
+      <c r="BC30" s="106"/>
+      <c r="BD30" s="106"/>
+      <c r="BE30" s="106"/>
+      <c r="BF30" s="106"/>
+      <c r="BG30" s="106"/>
+      <c r="BH30" s="106"/>
+      <c r="BI30" s="106"/>
+      <c r="BJ30" s="106"/>
+      <c r="BK30" s="106"/>
+      <c r="BL30" s="106"/>
+      <c r="BM30" s="106"/>
+      <c r="BN30" s="106"/>
+    </row>
+    <row r="31" spans="1:66" s="74" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A31" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="H31" s="62">
-        <v>0</v>
-      </c>
-      <c r="I31" s="63">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J31" s="94"/>
+      <c r="B31" s="71"/>
+      <c r="C31" s="72"/>
+      <c r="D31" s="72"/>
+      <c r="E31" s="103"/>
+      <c r="F31" s="103"/>
+      <c r="G31" s="73"/>
+      <c r="H31" s="73"/>
+      <c r="I31" s="73"/>
+      <c r="J31" s="97"/>
       <c r="K31" s="106"/>
       <c r="L31" s="106"/>
       <c r="M31" s="106"/>
@@ -6522,33 +6642,19 @@
       <c r="BM31" s="106"/>
       <c r="BN31" s="106"/>
     </row>
-    <row r="32" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A32" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>4.2</v>
-      </c>
-      <c r="B32" s="125" t="s">
-        <v>11</v>
-      </c>
-      <c r="D32" s="126"/>
-      <c r="E32" s="99">
-        <v>43130</v>
-      </c>
-      <c r="F32" s="100">
-        <f t="shared" si="6"/>
-        <v>43130</v>
-      </c>
-      <c r="G32" s="61">
-        <v>1</v>
-      </c>
-      <c r="H32" s="62">
-        <v>0</v>
-      </c>
-      <c r="I32" s="63">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J32" s="94"/>
+    <row r="32" spans="1:66" s="69" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A32" s="75" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="76"/>
+      <c r="C32" s="76"/>
+      <c r="D32" s="76"/>
+      <c r="E32" s="104"/>
+      <c r="F32" s="104"/>
+      <c r="G32" s="76"/>
+      <c r="H32" s="76"/>
+      <c r="I32" s="76"/>
+      <c r="J32" s="97"/>
       <c r="K32" s="106"/>
       <c r="L32" s="106"/>
       <c r="M32" s="106"/>
@@ -6606,33 +6712,28 @@
       <c r="BM32" s="106"/>
       <c r="BN32" s="106"/>
     </row>
-    <row r="33" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A33" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>4.3</v>
-      </c>
-      <c r="B33" s="125" t="s">
-        <v>11</v>
-      </c>
-      <c r="D33" s="126"/>
-      <c r="E33" s="99">
-        <v>43131</v>
-      </c>
-      <c r="F33" s="100">
-        <f t="shared" si="6"/>
-        <v>43131</v>
-      </c>
-      <c r="G33" s="61">
+    <row r="33" spans="1:66" s="69" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A33" s="128" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>1</v>
       </c>
-      <c r="H33" s="62">
-        <v>0</v>
-      </c>
-      <c r="I33" s="63">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J33" s="94"/>
+      <c r="B33" s="129" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" s="77"/>
+      <c r="D33" s="78"/>
+      <c r="E33" s="99"/>
+      <c r="F33" s="100" t="str">
+        <f t="shared" ref="F33:F36" si="9">IF(ISBLANK(E33)," - ",IF(G33=0,E33,E33+G33-1))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G33" s="61"/>
+      <c r="H33" s="62"/>
+      <c r="I33" s="79" t="str">
+        <f>IF(OR(F33=0,E33=0)," - ",NETWORKDAYS(E33,F33))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J33" s="98"/>
       <c r="K33" s="106"/>
       <c r="L33" s="106"/>
       <c r="M33" s="106"/>
@@ -6690,33 +6791,28 @@
       <c r="BM33" s="106"/>
       <c r="BN33" s="106"/>
     </row>
-    <row r="34" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:66" s="69" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" s="59" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>4.4</v>
-      </c>
-      <c r="B34" s="125" t="s">
-        <v>11</v>
-      </c>
-      <c r="D34" s="126"/>
-      <c r="E34" s="99">
-        <v>43132</v>
-      </c>
-      <c r="F34" s="100">
-        <f t="shared" si="6"/>
-        <v>43132</v>
-      </c>
-      <c r="G34" s="61">
-        <v>1</v>
-      </c>
-      <c r="H34" s="62">
-        <v>0</v>
-      </c>
-      <c r="I34" s="63">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J34" s="94"/>
+        <v>1.1</v>
+      </c>
+      <c r="B34" s="80" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="80"/>
+      <c r="D34" s="78"/>
+      <c r="E34" s="99"/>
+      <c r="F34" s="100" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G34" s="61"/>
+      <c r="H34" s="62"/>
+      <c r="I34" s="79" t="str">
+        <f t="shared" ref="I34:I36" si="10">IF(OR(F34=0,E34=0)," - ",NETWORKDAYS(E34,F34))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J34" s="98"/>
       <c r="K34" s="106"/>
       <c r="L34" s="106"/>
       <c r="M34" s="106"/>
@@ -6774,33 +6870,28 @@
       <c r="BM34" s="106"/>
       <c r="BN34" s="106"/>
     </row>
-    <row r="35" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:66" s="69" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>4.5</v>
-      </c>
-      <c r="B35" s="125" t="s">
-        <v>11</v>
-      </c>
-      <c r="D35" s="126"/>
-      <c r="E35" s="99">
-        <v>43133</v>
-      </c>
-      <c r="F35" s="100">
-        <f t="shared" si="6"/>
-        <v>43133</v>
-      </c>
-      <c r="G35" s="61">
-        <v>1</v>
-      </c>
-      <c r="H35" s="62">
-        <v>0</v>
-      </c>
-      <c r="I35" s="63">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J35" s="94"/>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <v>1.1.1</v>
+      </c>
+      <c r="B35" s="81" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" s="80"/>
+      <c r="D35" s="78"/>
+      <c r="E35" s="99"/>
+      <c r="F35" s="100" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G35" s="61"/>
+      <c r="H35" s="62"/>
+      <c r="I35" s="79" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J35" s="98"/>
       <c r="K35" s="106"/>
       <c r="L35" s="106"/>
       <c r="M35" s="106"/>
@@ -6859,19 +6950,27 @@
       <c r="BN35" s="106"/>
     </row>
     <row r="36" spans="1:66" s="69" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A36" s="59"/>
-      <c r="B36" s="64"/>
-      <c r="C36" s="64"/>
-      <c r="D36" s="65"/>
-      <c r="E36" s="102"/>
-      <c r="F36" s="102"/>
-      <c r="G36" s="66"/>
-      <c r="H36" s="67"/>
-      <c r="I36" s="68" t="str">
-        <f t="shared" si="4"/>
+      <c r="A36" s="59" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",4))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",3))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",4))-FIND("`",SUBSTITUTE(prevWBS,".","`",3))-1)))+1)))</f>
+        <v>1.1.1.1</v>
+      </c>
+      <c r="B36" s="81" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" s="80"/>
+      <c r="D36" s="78"/>
+      <c r="E36" s="99"/>
+      <c r="F36" s="100" t="str">
+        <f t="shared" si="9"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J36" s="96"/>
+      <c r="G36" s="61"/>
+      <c r="H36" s="62"/>
+      <c r="I36" s="79" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J36" s="98"/>
       <c r="K36" s="106"/>
       <c r="L36" s="106"/>
       <c r="M36" s="106"/>
@@ -6929,616 +7028,80 @@
       <c r="BM36" s="106"/>
       <c r="BN36" s="106"/>
     </row>
-    <row r="37" spans="1:66" s="69" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A37" s="59"/>
-      <c r="B37" s="64"/>
-      <c r="C37" s="64"/>
-      <c r="D37" s="65"/>
-      <c r="E37" s="102"/>
-      <c r="F37" s="102"/>
-      <c r="G37" s="66"/>
-      <c r="H37" s="67"/>
-      <c r="I37" s="68" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J37" s="96"/>
-      <c r="K37" s="106"/>
-      <c r="L37" s="106"/>
-      <c r="M37" s="106"/>
-      <c r="N37" s="106"/>
-      <c r="O37" s="106"/>
-      <c r="P37" s="106"/>
-      <c r="Q37" s="106"/>
-      <c r="R37" s="106"/>
-      <c r="S37" s="106"/>
-      <c r="T37" s="106"/>
-      <c r="U37" s="106"/>
-      <c r="V37" s="106"/>
-      <c r="W37" s="106"/>
-      <c r="X37" s="106"/>
-      <c r="Y37" s="106"/>
-      <c r="Z37" s="106"/>
-      <c r="AA37" s="106"/>
-      <c r="AB37" s="106"/>
-      <c r="AC37" s="106"/>
-      <c r="AD37" s="106"/>
-      <c r="AE37" s="106"/>
-      <c r="AF37" s="106"/>
-      <c r="AG37" s="106"/>
-      <c r="AH37" s="106"/>
-      <c r="AI37" s="106"/>
-      <c r="AJ37" s="106"/>
-      <c r="AK37" s="106"/>
-      <c r="AL37" s="106"/>
-      <c r="AM37" s="106"/>
-      <c r="AN37" s="106"/>
-      <c r="AO37" s="106"/>
-      <c r="AP37" s="106"/>
-      <c r="AQ37" s="106"/>
-      <c r="AR37" s="106"/>
-      <c r="AS37" s="106"/>
-      <c r="AT37" s="106"/>
-      <c r="AU37" s="106"/>
-      <c r="AV37" s="106"/>
-      <c r="AW37" s="106"/>
-      <c r="AX37" s="106"/>
-      <c r="AY37" s="106"/>
-      <c r="AZ37" s="106"/>
-      <c r="BA37" s="106"/>
-      <c r="BB37" s="106"/>
-      <c r="BC37" s="106"/>
-      <c r="BD37" s="106"/>
-      <c r="BE37" s="106"/>
-      <c r="BF37" s="106"/>
-      <c r="BG37" s="106"/>
-      <c r="BH37" s="106"/>
-      <c r="BI37" s="106"/>
-      <c r="BJ37" s="106"/>
-      <c r="BK37" s="106"/>
-      <c r="BL37" s="106"/>
-      <c r="BM37" s="106"/>
-      <c r="BN37" s="106"/>
-    </row>
-    <row r="38" spans="1:66" s="74" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A38" s="70" t="s">
-        <v>3</v>
-      </c>
-      <c r="B38" s="71"/>
-      <c r="C38" s="72"/>
-      <c r="D38" s="72"/>
-      <c r="E38" s="103"/>
-      <c r="F38" s="103"/>
-      <c r="G38" s="73"/>
-      <c r="H38" s="73"/>
-      <c r="I38" s="73"/>
-      <c r="J38" s="97"/>
-      <c r="K38" s="106"/>
-      <c r="L38" s="106"/>
-      <c r="M38" s="106"/>
-      <c r="N38" s="106"/>
-      <c r="O38" s="106"/>
-      <c r="P38" s="106"/>
-      <c r="Q38" s="106"/>
-      <c r="R38" s="106"/>
-      <c r="S38" s="106"/>
-      <c r="T38" s="106"/>
-      <c r="U38" s="106"/>
-      <c r="V38" s="106"/>
-      <c r="W38" s="106"/>
-      <c r="X38" s="106"/>
-      <c r="Y38" s="106"/>
-      <c r="Z38" s="106"/>
-      <c r="AA38" s="106"/>
-      <c r="AB38" s="106"/>
-      <c r="AC38" s="106"/>
-      <c r="AD38" s="106"/>
-      <c r="AE38" s="106"/>
-      <c r="AF38" s="106"/>
-      <c r="AG38" s="106"/>
-      <c r="AH38" s="106"/>
-      <c r="AI38" s="106"/>
-      <c r="AJ38" s="106"/>
-      <c r="AK38" s="106"/>
-      <c r="AL38" s="106"/>
-      <c r="AM38" s="106"/>
-      <c r="AN38" s="106"/>
-      <c r="AO38" s="106"/>
-      <c r="AP38" s="106"/>
-      <c r="AQ38" s="106"/>
-      <c r="AR38" s="106"/>
-      <c r="AS38" s="106"/>
-      <c r="AT38" s="106"/>
-      <c r="AU38" s="106"/>
-      <c r="AV38" s="106"/>
-      <c r="AW38" s="106"/>
-      <c r="AX38" s="106"/>
-      <c r="AY38" s="106"/>
-      <c r="AZ38" s="106"/>
-      <c r="BA38" s="106"/>
-      <c r="BB38" s="106"/>
-      <c r="BC38" s="106"/>
-      <c r="BD38" s="106"/>
-      <c r="BE38" s="106"/>
-      <c r="BF38" s="106"/>
-      <c r="BG38" s="106"/>
-      <c r="BH38" s="106"/>
-      <c r="BI38" s="106"/>
-      <c r="BJ38" s="106"/>
-      <c r="BK38" s="106"/>
-      <c r="BL38" s="106"/>
-      <c r="BM38" s="106"/>
-      <c r="BN38" s="106"/>
-    </row>
-    <row r="39" spans="1:66" s="69" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A39" s="75" t="s">
-        <v>42</v>
-      </c>
-      <c r="B39" s="76"/>
-      <c r="C39" s="76"/>
-      <c r="D39" s="76"/>
-      <c r="E39" s="104"/>
-      <c r="F39" s="104"/>
-      <c r="G39" s="76"/>
-      <c r="H39" s="76"/>
-      <c r="I39" s="76"/>
-      <c r="J39" s="97"/>
-      <c r="K39" s="106"/>
-      <c r="L39" s="106"/>
-      <c r="M39" s="106"/>
-      <c r="N39" s="106"/>
-      <c r="O39" s="106"/>
-      <c r="P39" s="106"/>
-      <c r="Q39" s="106"/>
-      <c r="R39" s="106"/>
-      <c r="S39" s="106"/>
-      <c r="T39" s="106"/>
-      <c r="U39" s="106"/>
-      <c r="V39" s="106"/>
-      <c r="W39" s="106"/>
-      <c r="X39" s="106"/>
-      <c r="Y39" s="106"/>
-      <c r="Z39" s="106"/>
-      <c r="AA39" s="106"/>
-      <c r="AB39" s="106"/>
-      <c r="AC39" s="106"/>
-      <c r="AD39" s="106"/>
-      <c r="AE39" s="106"/>
-      <c r="AF39" s="106"/>
-      <c r="AG39" s="106"/>
-      <c r="AH39" s="106"/>
-      <c r="AI39" s="106"/>
-      <c r="AJ39" s="106"/>
-      <c r="AK39" s="106"/>
-      <c r="AL39" s="106"/>
-      <c r="AM39" s="106"/>
-      <c r="AN39" s="106"/>
-      <c r="AO39" s="106"/>
-      <c r="AP39" s="106"/>
-      <c r="AQ39" s="106"/>
-      <c r="AR39" s="106"/>
-      <c r="AS39" s="106"/>
-      <c r="AT39" s="106"/>
-      <c r="AU39" s="106"/>
-      <c r="AV39" s="106"/>
-      <c r="AW39" s="106"/>
-      <c r="AX39" s="106"/>
-      <c r="AY39" s="106"/>
-      <c r="AZ39" s="106"/>
-      <c r="BA39" s="106"/>
-      <c r="BB39" s="106"/>
-      <c r="BC39" s="106"/>
-      <c r="BD39" s="106"/>
-      <c r="BE39" s="106"/>
-      <c r="BF39" s="106"/>
-      <c r="BG39" s="106"/>
-      <c r="BH39" s="106"/>
-      <c r="BI39" s="106"/>
-      <c r="BJ39" s="106"/>
-      <c r="BK39" s="106"/>
-      <c r="BL39" s="106"/>
-      <c r="BM39" s="106"/>
-      <c r="BN39" s="106"/>
-    </row>
-    <row r="40" spans="1:66" s="69" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A40" s="129" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>1</v>
-      </c>
-      <c r="B40" s="130" t="s">
-        <v>81</v>
-      </c>
-      <c r="C40" s="77"/>
-      <c r="D40" s="78"/>
-      <c r="E40" s="99"/>
-      <c r="F40" s="100" t="str">
-        <f t="shared" ref="F40:F43" si="7">IF(ISBLANK(E40)," - ",IF(G40=0,E40,E40+G40-1))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G40" s="61"/>
-      <c r="H40" s="62"/>
-      <c r="I40" s="79" t="str">
-        <f>IF(OR(F40=0,E40=0)," - ",NETWORKDAYS(E40,F40))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J40" s="98"/>
-      <c r="K40" s="106"/>
-      <c r="L40" s="106"/>
-      <c r="M40" s="106"/>
-      <c r="N40" s="106"/>
-      <c r="O40" s="106"/>
-      <c r="P40" s="106"/>
-      <c r="Q40" s="106"/>
-      <c r="R40" s="106"/>
-      <c r="S40" s="106"/>
-      <c r="T40" s="106"/>
-      <c r="U40" s="106"/>
-      <c r="V40" s="106"/>
-      <c r="W40" s="106"/>
-      <c r="X40" s="106"/>
-      <c r="Y40" s="106"/>
-      <c r="Z40" s="106"/>
-      <c r="AA40" s="106"/>
-      <c r="AB40" s="106"/>
-      <c r="AC40" s="106"/>
-      <c r="AD40" s="106"/>
-      <c r="AE40" s="106"/>
-      <c r="AF40" s="106"/>
-      <c r="AG40" s="106"/>
-      <c r="AH40" s="106"/>
-      <c r="AI40" s="106"/>
-      <c r="AJ40" s="106"/>
-      <c r="AK40" s="106"/>
-      <c r="AL40" s="106"/>
-      <c r="AM40" s="106"/>
-      <c r="AN40" s="106"/>
-      <c r="AO40" s="106"/>
-      <c r="AP40" s="106"/>
-      <c r="AQ40" s="106"/>
-      <c r="AR40" s="106"/>
-      <c r="AS40" s="106"/>
-      <c r="AT40" s="106"/>
-      <c r="AU40" s="106"/>
-      <c r="AV40" s="106"/>
-      <c r="AW40" s="106"/>
-      <c r="AX40" s="106"/>
-      <c r="AY40" s="106"/>
-      <c r="AZ40" s="106"/>
-      <c r="BA40" s="106"/>
-      <c r="BB40" s="106"/>
-      <c r="BC40" s="106"/>
-      <c r="BD40" s="106"/>
-      <c r="BE40" s="106"/>
-      <c r="BF40" s="106"/>
-      <c r="BG40" s="106"/>
-      <c r="BH40" s="106"/>
-      <c r="BI40" s="106"/>
-      <c r="BJ40" s="106"/>
-      <c r="BK40" s="106"/>
-      <c r="BL40" s="106"/>
-      <c r="BM40" s="106"/>
-      <c r="BN40" s="106"/>
-    </row>
-    <row r="41" spans="1:66" s="69" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A41" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>1.1</v>
-      </c>
-      <c r="B41" s="80" t="s">
-        <v>67</v>
-      </c>
-      <c r="C41" s="80"/>
-      <c r="D41" s="78"/>
-      <c r="E41" s="99"/>
-      <c r="F41" s="100" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G41" s="61"/>
-      <c r="H41" s="62"/>
-      <c r="I41" s="79" t="str">
-        <f t="shared" ref="I41:I43" si="8">IF(OR(F41=0,E41=0)," - ",NETWORKDAYS(E41,F41))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J41" s="98"/>
-      <c r="K41" s="106"/>
-      <c r="L41" s="106"/>
-      <c r="M41" s="106"/>
-      <c r="N41" s="106"/>
-      <c r="O41" s="106"/>
-      <c r="P41" s="106"/>
-      <c r="Q41" s="106"/>
-      <c r="R41" s="106"/>
-      <c r="S41" s="106"/>
-      <c r="T41" s="106"/>
-      <c r="U41" s="106"/>
-      <c r="V41" s="106"/>
-      <c r="W41" s="106"/>
-      <c r="X41" s="106"/>
-      <c r="Y41" s="106"/>
-      <c r="Z41" s="106"/>
-      <c r="AA41" s="106"/>
-      <c r="AB41" s="106"/>
-      <c r="AC41" s="106"/>
-      <c r="AD41" s="106"/>
-      <c r="AE41" s="106"/>
-      <c r="AF41" s="106"/>
-      <c r="AG41" s="106"/>
-      <c r="AH41" s="106"/>
-      <c r="AI41" s="106"/>
-      <c r="AJ41" s="106"/>
-      <c r="AK41" s="106"/>
-      <c r="AL41" s="106"/>
-      <c r="AM41" s="106"/>
-      <c r="AN41" s="106"/>
-      <c r="AO41" s="106"/>
-      <c r="AP41" s="106"/>
-      <c r="AQ41" s="106"/>
-      <c r="AR41" s="106"/>
-      <c r="AS41" s="106"/>
-      <c r="AT41" s="106"/>
-      <c r="AU41" s="106"/>
-      <c r="AV41" s="106"/>
-      <c r="AW41" s="106"/>
-      <c r="AX41" s="106"/>
-      <c r="AY41" s="106"/>
-      <c r="AZ41" s="106"/>
-      <c r="BA41" s="106"/>
-      <c r="BB41" s="106"/>
-      <c r="BC41" s="106"/>
-      <c r="BD41" s="106"/>
-      <c r="BE41" s="106"/>
-      <c r="BF41" s="106"/>
-      <c r="BG41" s="106"/>
-      <c r="BH41" s="106"/>
-      <c r="BI41" s="106"/>
-      <c r="BJ41" s="106"/>
-      <c r="BK41" s="106"/>
-      <c r="BL41" s="106"/>
-      <c r="BM41" s="106"/>
-      <c r="BN41" s="106"/>
-    </row>
-    <row r="42" spans="1:66" s="69" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A42" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
-        <v>1.1.1</v>
-      </c>
-      <c r="B42" s="81" t="s">
-        <v>68</v>
-      </c>
-      <c r="C42" s="80"/>
-      <c r="D42" s="78"/>
-      <c r="E42" s="99"/>
-      <c r="F42" s="100" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G42" s="61"/>
-      <c r="H42" s="62"/>
-      <c r="I42" s="79" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J42" s="98"/>
-      <c r="K42" s="106"/>
-      <c r="L42" s="106"/>
-      <c r="M42" s="106"/>
-      <c r="N42" s="106"/>
-      <c r="O42" s="106"/>
-      <c r="P42" s="106"/>
-      <c r="Q42" s="106"/>
-      <c r="R42" s="106"/>
-      <c r="S42" s="106"/>
-      <c r="T42" s="106"/>
-      <c r="U42" s="106"/>
-      <c r="V42" s="106"/>
-      <c r="W42" s="106"/>
-      <c r="X42" s="106"/>
-      <c r="Y42" s="106"/>
-      <c r="Z42" s="106"/>
-      <c r="AA42" s="106"/>
-      <c r="AB42" s="106"/>
-      <c r="AC42" s="106"/>
-      <c r="AD42" s="106"/>
-      <c r="AE42" s="106"/>
-      <c r="AF42" s="106"/>
-      <c r="AG42" s="106"/>
-      <c r="AH42" s="106"/>
-      <c r="AI42" s="106"/>
-      <c r="AJ42" s="106"/>
-      <c r="AK42" s="106"/>
-      <c r="AL42" s="106"/>
-      <c r="AM42" s="106"/>
-      <c r="AN42" s="106"/>
-      <c r="AO42" s="106"/>
-      <c r="AP42" s="106"/>
-      <c r="AQ42" s="106"/>
-      <c r="AR42" s="106"/>
-      <c r="AS42" s="106"/>
-      <c r="AT42" s="106"/>
-      <c r="AU42" s="106"/>
-      <c r="AV42" s="106"/>
-      <c r="AW42" s="106"/>
-      <c r="AX42" s="106"/>
-      <c r="AY42" s="106"/>
-      <c r="AZ42" s="106"/>
-      <c r="BA42" s="106"/>
-      <c r="BB42" s="106"/>
-      <c r="BC42" s="106"/>
-      <c r="BD42" s="106"/>
-      <c r="BE42" s="106"/>
-      <c r="BF42" s="106"/>
-      <c r="BG42" s="106"/>
-      <c r="BH42" s="106"/>
-      <c r="BI42" s="106"/>
-      <c r="BJ42" s="106"/>
-      <c r="BK42" s="106"/>
-      <c r="BL42" s="106"/>
-      <c r="BM42" s="106"/>
-      <c r="BN42" s="106"/>
-    </row>
-    <row r="43" spans="1:66" s="69" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A43" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",4))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",3))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",4))-FIND("`",SUBSTITUTE(prevWBS,".","`",3))-1)))+1)))</f>
-        <v>1.1.1.1</v>
-      </c>
-      <c r="B43" s="81" t="s">
-        <v>69</v>
-      </c>
-      <c r="C43" s="80"/>
-      <c r="D43" s="78"/>
-      <c r="E43" s="99"/>
-      <c r="F43" s="100" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G43" s="61"/>
-      <c r="H43" s="62"/>
-      <c r="I43" s="79" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J43" s="98"/>
-      <c r="K43" s="106"/>
-      <c r="L43" s="106"/>
-      <c r="M43" s="106"/>
-      <c r="N43" s="106"/>
-      <c r="O43" s="106"/>
-      <c r="P43" s="106"/>
-      <c r="Q43" s="106"/>
-      <c r="R43" s="106"/>
-      <c r="S43" s="106"/>
-      <c r="T43" s="106"/>
-      <c r="U43" s="106"/>
-      <c r="V43" s="106"/>
-      <c r="W43" s="106"/>
-      <c r="X43" s="106"/>
-      <c r="Y43" s="106"/>
-      <c r="Z43" s="106"/>
-      <c r="AA43" s="106"/>
-      <c r="AB43" s="106"/>
-      <c r="AC43" s="106"/>
-      <c r="AD43" s="106"/>
-      <c r="AE43" s="106"/>
-      <c r="AF43" s="106"/>
-      <c r="AG43" s="106"/>
-      <c r="AH43" s="106"/>
-      <c r="AI43" s="106"/>
-      <c r="AJ43" s="106"/>
-      <c r="AK43" s="106"/>
-      <c r="AL43" s="106"/>
-      <c r="AM43" s="106"/>
-      <c r="AN43" s="106"/>
-      <c r="AO43" s="106"/>
-      <c r="AP43" s="106"/>
-      <c r="AQ43" s="106"/>
-      <c r="AR43" s="106"/>
-      <c r="AS43" s="106"/>
-      <c r="AT43" s="106"/>
-      <c r="AU43" s="106"/>
-      <c r="AV43" s="106"/>
-      <c r="AW43" s="106"/>
-      <c r="AX43" s="106"/>
-      <c r="AY43" s="106"/>
-      <c r="AZ43" s="106"/>
-      <c r="BA43" s="106"/>
-      <c r="BB43" s="106"/>
-      <c r="BC43" s="106"/>
-      <c r="BD43" s="106"/>
-      <c r="BE43" s="106"/>
-      <c r="BF43" s="106"/>
-      <c r="BG43" s="106"/>
-      <c r="BH43" s="106"/>
-      <c r="BI43" s="106"/>
-      <c r="BJ43" s="106"/>
-      <c r="BK43" s="106"/>
-      <c r="BL43" s="106"/>
-      <c r="BM43" s="106"/>
-      <c r="BN43" s="106"/>
-    </row>
-    <row r="44" spans="1:66" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="172" t="str">
+    <row r="37" spans="1:66" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="161" t="str">
         <f>HYPERLINK("https://vertex42.link/HowToCreateAGanttChart","► Watch How to Create a Gantt Chart in Excel")</f>
         <v>► Watch How to Create a Gantt Chart in Excel</v>
       </c>
-      <c r="B44" s="30"/>
-      <c r="C44" s="30"/>
-      <c r="D44" s="31"/>
-      <c r="E44" s="30"/>
-      <c r="F44" s="30"/>
-      <c r="G44" s="30"/>
-      <c r="H44" s="30"/>
-      <c r="I44" s="30"/>
-      <c r="J44" s="30"/>
-      <c r="K44" s="30"/>
-      <c r="L44" s="30"/>
-      <c r="M44" s="30"/>
-      <c r="N44" s="30"/>
-      <c r="O44" s="30"/>
-      <c r="P44" s="30"/>
-      <c r="Q44" s="30"/>
-      <c r="R44" s="30"/>
-      <c r="S44" s="30"/>
-      <c r="T44" s="30"/>
-      <c r="U44" s="30"/>
-      <c r="V44" s="30"/>
-      <c r="W44" s="30"/>
-      <c r="X44" s="30"/>
-      <c r="Y44" s="30"/>
-      <c r="Z44" s="30"/>
-      <c r="AA44" s="30"/>
-      <c r="AB44" s="30"/>
-      <c r="AC44" s="30"/>
-      <c r="AD44" s="30"/>
-      <c r="AE44" s="30"/>
-      <c r="AF44" s="30"/>
-      <c r="AG44" s="30"/>
-      <c r="AH44" s="30"/>
-      <c r="AI44" s="30"/>
-      <c r="AJ44" s="30"/>
-      <c r="AK44" s="30"/>
-      <c r="AL44" s="30"/>
-      <c r="AM44" s="30"/>
-      <c r="AN44" s="30"/>
-      <c r="AO44" s="30"/>
-      <c r="AP44" s="30"/>
-      <c r="AQ44" s="30"/>
-      <c r="AR44" s="30"/>
-      <c r="AS44" s="30"/>
-      <c r="AT44" s="30"/>
-      <c r="AU44" s="30"/>
-      <c r="AV44" s="30"/>
-      <c r="AW44" s="30"/>
-      <c r="AX44" s="30"/>
-      <c r="AY44" s="30"/>
-      <c r="AZ44" s="30"/>
-      <c r="BA44" s="30"/>
-      <c r="BB44" s="30"/>
-      <c r="BC44" s="30"/>
-      <c r="BD44" s="30"/>
-      <c r="BE44" s="30"/>
-      <c r="BF44" s="30"/>
-      <c r="BG44" s="30"/>
-      <c r="BH44" s="30"/>
-      <c r="BI44" s="30"/>
-      <c r="BJ44" s="30"/>
-      <c r="BK44" s="30"/>
-      <c r="BL44" s="30"/>
-      <c r="BM44" s="30"/>
-      <c r="BN44" s="30"/>
+      <c r="B37" s="30"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="30"/>
+      <c r="I37" s="30"/>
+      <c r="J37" s="30"/>
+      <c r="K37" s="30"/>
+      <c r="L37" s="30"/>
+      <c r="M37" s="30"/>
+      <c r="N37" s="30"/>
+      <c r="O37" s="30"/>
+      <c r="P37" s="30"/>
+      <c r="Q37" s="30"/>
+      <c r="R37" s="30"/>
+      <c r="S37" s="30"/>
+      <c r="T37" s="30"/>
+      <c r="U37" s="30"/>
+      <c r="V37" s="30"/>
+      <c r="W37" s="30"/>
+      <c r="X37" s="30"/>
+      <c r="Y37" s="30"/>
+      <c r="Z37" s="30"/>
+      <c r="AA37" s="30"/>
+      <c r="AB37" s="30"/>
+      <c r="AC37" s="30"/>
+      <c r="AD37" s="30"/>
+      <c r="AE37" s="30"/>
+      <c r="AF37" s="30"/>
+      <c r="AG37" s="30"/>
+      <c r="AH37" s="30"/>
+      <c r="AI37" s="30"/>
+      <c r="AJ37" s="30"/>
+      <c r="AK37" s="30"/>
+      <c r="AL37" s="30"/>
+      <c r="AM37" s="30"/>
+      <c r="AN37" s="30"/>
+      <c r="AO37" s="30"/>
+      <c r="AP37" s="30"/>
+      <c r="AQ37" s="30"/>
+      <c r="AR37" s="30"/>
+      <c r="AS37" s="30"/>
+      <c r="AT37" s="30"/>
+      <c r="AU37" s="30"/>
+      <c r="AV37" s="30"/>
+      <c r="AW37" s="30"/>
+      <c r="AX37" s="30"/>
+      <c r="AY37" s="30"/>
+      <c r="AZ37" s="30"/>
+      <c r="BA37" s="30"/>
+      <c r="BB37" s="30"/>
+      <c r="BC37" s="30"/>
+      <c r="BD37" s="30"/>
+      <c r="BE37" s="30"/>
+      <c r="BF37" s="30"/>
+      <c r="BG37" s="30"/>
+      <c r="BH37" s="30"/>
+      <c r="BI37" s="30"/>
+      <c r="BJ37" s="30"/>
+      <c r="BK37" s="30"/>
+      <c r="BL37" s="30"/>
+      <c r="BM37" s="30"/>
+      <c r="BN37" s="30"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -7549,10 +7112,19 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="H8:H43">
-    <cfRule type="dataBar" priority="2">
+  <conditionalFormatting sqref="H8:H13 H15:H36">
+    <cfRule type="dataBar" priority="10">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7566,20 +7138,47 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:BN7">
-    <cfRule type="expression" dxfId="3" priority="45">
+    <cfRule type="expression" dxfId="6" priority="53">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K8:BN43">
-    <cfRule type="expression" dxfId="2" priority="48">
+  <conditionalFormatting sqref="K8:BN13 K15:BN36">
+    <cfRule type="expression" dxfId="5" priority="56">
       <formula>AND($E8&lt;=K$6,ROUNDDOWN(($F8-$E8+1)*$H8,0)+$E8-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="49">
+    <cfRule type="expression" dxfId="4" priority="57">
       <formula>AND(NOT(ISBLANK($E8)),$E8&lt;=K$6,$F8&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K6:BN43">
-    <cfRule type="expression" dxfId="0" priority="8">
+  <conditionalFormatting sqref="K6:BN13 K15:BN36">
+    <cfRule type="expression" dxfId="3" priority="16">
+      <formula>K$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H14">
+    <cfRule type="dataBar" priority="5">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{8B894183-9857-4A8A-A710-A8E0A3639C63}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K14:BN14">
+    <cfRule type="expression" dxfId="2" priority="7">
+      <formula>AND($E14&lt;=K$6,ROUNDDOWN(($F14-$E14+1)*$H14,0)+$E14-1&gt;=K$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="8">
+      <formula>AND(NOT(ISBLANK($E14)),$E14&lt;=K$6,$F14&gt;=K$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K14:BN14">
+    <cfRule type="expression" dxfId="0" priority="6">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7593,8 +7192,8 @@
   <pageSetup scale="63" fitToHeight="0" orientation="landscape" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
-    <ignoredError sqref="H9 A36:B37 B31 B32:B34 B25:B28 B19:B22 G13:H13 G12 G16 G14:H14 A39:B39 B38 E18 E24 E30 E36:H39 G15 G11 G10 G18:H18 G24:H24 G30:H34 H22 G40 G41:G42 G43 H20 H21 H25:H28" unlockedFormula="1"/>
-    <ignoredError sqref="A30 A24 A18" formula="1"/>
+    <ignoredError sqref="H9 A29:B30 B24 B25:B27 A32:B32 B31 E23 E29:H32 H12 H16 G23:H27 G33 G34:G35 G36 H18 H20" unlockedFormula="1"/>
+    <ignoredError sqref="A23 A16 A12" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId3"/>
   <legacyDrawing r:id="rId4"/>
@@ -7642,7 +7241,22 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H8:H43</xm:sqref>
+          <xm:sqref>H8:H13 H15:H36</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{8B894183-9857-4A8A-A710-A8E0A3639C63}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H14</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -7671,17 +7285,17 @@
   <sheetData>
     <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="34" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C4" s="23" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C5" s="20" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -7689,149 +7303,149 @@
     </row>
     <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="C7" s="24" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C8" s="25" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C10" s="20" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C11" s="20" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="C13" s="24" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="18" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" s="26" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="20" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="2:2" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B22" s="26" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B23" s="20" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B24" s="20" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="2:2" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B26" s="26" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B27" s="20" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B28" s="20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B29" s="20" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B30" s="16" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B31" s="16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B32" s="16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B34" s="26" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" s="20" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B36" s="20" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B37" s="20" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="39" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B39" s="26" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B40" s="20" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="2:2" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B42" s="26" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="43" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B43" s="20" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="44" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B44" s="20" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="45" spans="2:2" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="46" spans="2:2" ht="18" x14ac:dyDescent="0.25">
       <c r="B46" s="24" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -7865,14 +7479,14 @@
   <sheetData>
     <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="39" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B1" s="40"/>
       <c r="C1" s="41"/>
     </row>
     <row r="2" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="137" t="s">
-        <v>53</v>
+      <c r="A2" s="136" t="s">
+        <v>50</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="8"/>
@@ -7883,208 +7497,208 @@
       <c r="C3" s="8"/>
     </row>
     <row r="4" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A4" s="132" t="s">
-        <v>94</v>
+      <c r="A4" s="131" t="s">
+        <v>91</v>
       </c>
       <c r="B4" s="38"/>
     </row>
     <row r="5" spans="1:3" s="8" customFormat="1" ht="57" x14ac:dyDescent="0.2">
-      <c r="B5" s="138" t="s">
-        <v>83</v>
+      <c r="B5" s="137" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B7" s="138" t="s">
-        <v>95</v>
+      <c r="B7" s="137" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B9" s="137" t="s">
-        <v>65</v>
+      <c r="B9" s="136" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B11" s="136" t="s">
-        <v>66</v>
+      <c r="B11" s="135" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="171" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B13" s="171"/>
     </row>
     <row r="14" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:3" s="133" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A15" s="141"/>
-      <c r="B15" s="139" t="s">
+    <row r="15" spans="1:3" s="132" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15" s="140"/>
+      <c r="B15" s="138" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="132" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A16" s="140"/>
+      <c r="B16" s="139" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="134" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A17" s="141"/>
+      <c r="B17" s="139" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A18" s="141"/>
+      <c r="B18" s="139" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="41" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A19" s="144"/>
+      <c r="B19" s="139" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="132" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A20" s="140"/>
+      <c r="B20" s="138" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="133" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A21" s="141"/>
+      <c r="B21" s="139" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A22" s="142"/>
+      <c r="B22" s="143" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="133" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A16" s="141"/>
-      <c r="B16" s="140" t="s">
-        <v>84</v>
-      </c>
-      <c r="C16" s="135" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A17" s="142"/>
-      <c r="B17" s="140" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A18" s="142"/>
-      <c r="B18" s="140" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" s="41" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="145"/>
-      <c r="B19" s="140" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" s="133" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A20" s="141"/>
-      <c r="B20" s="139" t="s">
-        <v>85</v>
-      </c>
-      <c r="C20" s="134" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A21" s="142"/>
-      <c r="B21" s="140" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A22" s="143"/>
-      <c r="B22" s="144" t="s">
-        <v>89</v>
-      </c>
-    </row>
     <row r="23" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A23" s="143"/>
+      <c r="A23" s="142"/>
       <c r="B23" s="10"/>
     </row>
     <row r="24" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="171" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" s="171"/>
+    </row>
+    <row r="25" spans="1:3" s="8" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="142"/>
+      <c r="B25" s="139" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A26" s="142"/>
+      <c r="B26" s="139"/>
+    </row>
+    <row r="27" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A27" s="142"/>
+      <c r="B27" s="160" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A28" s="142"/>
+      <c r="B28" s="139" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="142"/>
+      <c r="B29" s="139" t="s">
         <v>90</v>
       </c>
-      <c r="B24" s="171"/>
-    </row>
-    <row r="25" spans="1:3" s="8" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="143"/>
-      <c r="B25" s="140" t="s">
+    </row>
+    <row r="30" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A30" s="142"/>
+      <c r="B30" s="139"/>
+    </row>
+    <row r="31" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A31" s="142"/>
+      <c r="B31" s="160" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A32" s="142"/>
+      <c r="B32" s="139" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A33" s="142"/>
+      <c r="B33" s="139" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A34" s="142"/>
+      <c r="B34" s="10"/>
+    </row>
+    <row r="35" spans="1:2" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A35" s="142"/>
+      <c r="B35" s="139" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A36" s="142"/>
+      <c r="B36" s="145" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A26" s="143"/>
-      <c r="B26" s="140"/>
-    </row>
-    <row r="27" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A27" s="143"/>
-      <c r="B27" s="161" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A28" s="143"/>
-      <c r="B28" s="140" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="143"/>
-      <c r="B29" s="140" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A30" s="143"/>
-      <c r="B30" s="140"/>
-    </row>
-    <row r="31" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A31" s="143"/>
-      <c r="B31" s="161" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A32" s="143"/>
-      <c r="B32" s="140" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A33" s="143"/>
-      <c r="B33" s="140" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A34" s="143"/>
-      <c r="B34" s="10"/>
-    </row>
-    <row r="35" spans="1:2" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="143"/>
-      <c r="B35" s="140" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A36" s="143"/>
-      <c r="B36" s="146" t="s">
-        <v>101</v>
-      </c>
-    </row>
     <row r="37" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A37" s="143"/>
+      <c r="A37" s="142"/>
       <c r="B37" s="10"/>
     </row>
     <row r="38" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A38" s="171" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B38" s="171"/>
     </row>
     <row r="39" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B39" s="140" t="s">
-        <v>104</v>
+      <c r="B39" s="139" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="41" spans="1:2" s="20" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B41" s="140" t="s">
-        <v>105</v>
+      <c r="B41" s="139" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="42" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="43" spans="1:2" s="20" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B43" s="140" t="s">
-        <v>103</v>
+      <c r="B43" s="139" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="45" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B45" s="140" t="s">
-        <v>106</v>
+      <c r="B45" s="139" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B46" s="21"/>
     </row>
     <row r="47" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B47" s="140" t="s">
-        <v>107</v>
+      <c r="B47" s="139" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -8092,100 +7706,100 @@
     </row>
     <row r="49" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A49" s="171" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B49" s="171"/>
     </row>
     <row r="50" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B50" s="140" t="s">
-        <v>139</v>
+      <c r="B50" s="139" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B51" s="11"/>
     </row>
     <row r="52" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A52" s="147" t="s">
+      <c r="A52" s="146" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" s="139" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A53" s="146" t="s">
+        <v>14</v>
+      </c>
+      <c r="B53" s="139" t="s">
         <v>15</v>
       </c>
-      <c r="B52" s="140" t="s">
+    </row>
+    <row r="54" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A54" s="146" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A53" s="147" t="s">
+      <c r="B54" s="139" t="s">
         <v>17</v>
       </c>
-      <c r="B53" s="140" t="s">
+    </row>
+    <row r="55" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A55" s="135"/>
+      <c r="B55" s="139" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A56" s="135"/>
+      <c r="B56" s="139" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A57" s="146" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A54" s="147" t="s">
+      <c r="B57" s="139" t="s">
         <v>19</v>
       </c>
-      <c r="B54" s="140" t="s">
+    </row>
+    <row r="58" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A58" s="135"/>
+      <c r="B58" s="139" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A59" s="135"/>
+      <c r="B59" s="139" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A60" s="146" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A55" s="136"/>
-      <c r="B55" s="140" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A56" s="136"/>
-      <c r="B56" s="140" t="s">
+      <c r="B60" s="139" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A61" s="135"/>
+      <c r="B61" s="139" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A57" s="147" t="s">
-        <v>21</v>
-      </c>
-      <c r="B57" s="140" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A58" s="136"/>
-      <c r="B58" s="140" t="s">
+    <row r="62" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A62" s="146" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A59" s="136"/>
-      <c r="B59" s="140" t="s">
+      <c r="B62" s="139" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A60" s="147" t="s">
-        <v>23</v>
-      </c>
-      <c r="B60" s="140" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A61" s="136"/>
-      <c r="B61" s="140" t="s">
+    <row r="63" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A63" s="147"/>
+      <c r="B63" s="139" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A62" s="147" t="s">
-        <v>113</v>
-      </c>
-      <c r="B62" s="140" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A63" s="148"/>
-      <c r="B63" s="140" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="64" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
@@ -8193,13 +7807,13 @@
     </row>
     <row r="65" spans="1:2" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A65" s="171" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B65" s="171"/>
     </row>
     <row r="66" spans="1:2" s="20" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="B66" s="140" t="s">
-        <v>116</v>
+      <c r="B66" s="139" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="67" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
@@ -8207,159 +7821,159 @@
     </row>
     <row r="68" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A68" s="171" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B68" s="171"/>
     </row>
     <row r="69" spans="1:2" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A69" s="155" t="s">
-        <v>8</v>
-      </c>
-      <c r="B69" s="156" t="s">
+      <c r="A69" s="154" t="s">
+        <v>6</v>
+      </c>
+      <c r="B69" s="155" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A70" s="148"/>
+      <c r="B70" s="153" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A71" s="148"/>
+      <c r="B71" s="149"/>
+    </row>
+    <row r="72" spans="1:2" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A72" s="154" t="s">
+        <v>6</v>
+      </c>
+      <c r="B72" s="155" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A73" s="148"/>
+      <c r="B73" s="153" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A74" s="148"/>
+      <c r="B74" s="149"/>
+    </row>
+    <row r="75" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A75" s="154" t="s">
+        <v>6</v>
+      </c>
+      <c r="B75" s="157" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" s="8" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A76" s="148"/>
+      <c r="B76" s="137" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A77" s="147"/>
+      <c r="B77" s="147"/>
+    </row>
+    <row r="78" spans="1:2" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A78" s="154" t="s">
+        <v>6</v>
+      </c>
+      <c r="B78" s="157" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A79" s="148"/>
+      <c r="B79" s="137" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" s="20" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A80" s="147"/>
+      <c r="B80" s="147"/>
+    </row>
+    <row r="81" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A81" s="154" t="s">
+        <v>6</v>
+      </c>
+      <c r="B81" s="157" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A82" s="148"/>
+      <c r="B82" s="152" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A83" s="148"/>
+      <c r="B83" s="152" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A84" s="148"/>
+      <c r="B84" s="152" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A85" s="147"/>
+      <c r="B85" s="151"/>
+    </row>
+    <row r="86" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A86" s="154" t="s">
+        <v>6</v>
+      </c>
+      <c r="B86" s="157" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" s="8" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A87" s="148"/>
+      <c r="B87" s="137" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A88" s="148"/>
+      <c r="B88" s="150" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="70" spans="1:2" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A70" s="149"/>
-      <c r="B70" s="154" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A71" s="149"/>
-      <c r="B71" s="150"/>
-    </row>
-    <row r="72" spans="1:2" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A72" s="155" t="s">
-        <v>8</v>
-      </c>
-      <c r="B72" s="156" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A73" s="149"/>
-      <c r="B73" s="154" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A74" s="149"/>
-      <c r="B74" s="150"/>
-    </row>
-    <row r="75" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A75" s="155" t="s">
-        <v>8</v>
-      </c>
-      <c r="B75" s="158" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" s="8" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A76" s="149"/>
-      <c r="B76" s="138" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A77" s="148"/>
-      <c r="B77" s="148"/>
-    </row>
-    <row r="78" spans="1:2" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A78" s="155" t="s">
-        <v>8</v>
-      </c>
-      <c r="B78" s="158" t="s">
+    <row r="89" spans="1:2" s="8" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+      <c r="A89" s="148"/>
+      <c r="B89" s="156" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A90" s="147"/>
+      <c r="B90" s="147"/>
+    </row>
+    <row r="91" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A91" s="154" t="s">
+        <v>6</v>
+      </c>
+      <c r="B91" s="159" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="79" spans="1:2" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A79" s="149"/>
-      <c r="B79" s="138" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" s="20" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A80" s="148"/>
-      <c r="B80" s="148"/>
-    </row>
-    <row r="81" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A81" s="155" t="s">
-        <v>8</v>
-      </c>
-      <c r="B81" s="158" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A82" s="149"/>
-      <c r="B82" s="153" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A83" s="149"/>
-      <c r="B83" s="153" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A84" s="149"/>
-      <c r="B84" s="153" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A85" s="148"/>
-      <c r="B85" s="152"/>
-    </row>
-    <row r="86" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A86" s="155" t="s">
-        <v>8</v>
-      </c>
-      <c r="B86" s="158" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" s="8" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A87" s="149"/>
-      <c r="B87" s="138" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A88" s="149"/>
-      <c r="B88" s="151" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" s="8" customFormat="1" ht="57" x14ac:dyDescent="0.2">
-      <c r="A89" s="149"/>
-      <c r="B89" s="157" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A90" s="148"/>
-      <c r="B90" s="148"/>
-    </row>
-    <row r="91" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A91" s="155" t="s">
-        <v>8</v>
-      </c>
-      <c r="B91" s="160" t="s">
-        <v>131</v>
-      </c>
-    </row>
     <row r="92" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A92" s="136"/>
-      <c r="B92" s="153" t="s">
-        <v>25</v>
+      <c r="A92" s="135"/>
+      <c r="B92" s="152" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="28" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -8402,7 +8016,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="39" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B1" s="39"/>
       <c r="C1" s="44"/>
@@ -8417,14 +8031,14 @@
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="42"/>
       <c r="B3" s="35" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C3" s="43"/>
     </row>
     <row r="4" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="14"/>
       <c r="B4" s="37" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C4" s="15"/>
     </row>
@@ -8436,7 +8050,7 @@
     <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="18" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C6" s="15"/>
     </row>
@@ -8448,7 +8062,7 @@
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="14"/>
       <c r="B8" s="17" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C8" s="15"/>
     </row>
@@ -8460,7 +8074,7 @@
     <row r="10" spans="1:4" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
       <c r="B10" s="17" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C10" s="15"/>
     </row>
@@ -8472,7 +8086,7 @@
     <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A12" s="14"/>
       <c r="B12" s="17" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C12" s="15"/>
     </row>
@@ -8484,7 +8098,7 @@
     <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A14" s="14"/>
       <c r="B14" s="17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C14" s="15"/>
     </row>
@@ -8496,7 +8110,7 @@
     <row r="16" spans="1:4" ht="30.75" x14ac:dyDescent="0.2">
       <c r="A16" s="14"/>
       <c r="B16" s="17" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C16" s="15"/>
     </row>
@@ -8508,14 +8122,14 @@
     <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="18" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C18" s="15"/>
     </row>
     <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="14"/>
       <c r="B19" s="36" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C19" s="15"/>
     </row>

</xml_diff>

<commit_message>
docs (mockup): buat navbar dan home page
</commit_message>
<xml_diff>
--- a/Gantt Chart.xlsx
+++ b/Gantt Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\punch\Documents\GitHub\warawiriweb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{963D25DB-5EFA-4DFD-B2E6-A7A172356C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4270268A-4171-42BE-9F46-CD19E77C6C4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2945,6 +2945,45 @@
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="34" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="47" fillId="25" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="47" fillId="26" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="47" fillId="26" borderId="0" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="54" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2952,51 +2991,12 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="45" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="47" fillId="25" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="47" fillId="26" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="47" fillId="26" borderId="0" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="54" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3856,7 +3856,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AY13" sqref="AY13"/>
+      <selection pane="bottomLeft" activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3884,29 +3884,29 @@
       <c r="E1" s="46"/>
       <c r="F1" s="46"/>
       <c r="I1" s="130"/>
-      <c r="K1" s="162" t="s">
+      <c r="K1" s="175" t="s">
         <v>79</v>
       </c>
-      <c r="L1" s="162"/>
-      <c r="M1" s="162"/>
-      <c r="N1" s="162"/>
-      <c r="O1" s="162"/>
-      <c r="P1" s="162"/>
-      <c r="Q1" s="162"/>
-      <c r="R1" s="162"/>
-      <c r="S1" s="162"/>
-      <c r="T1" s="162"/>
-      <c r="U1" s="162"/>
-      <c r="V1" s="162"/>
-      <c r="W1" s="162"/>
-      <c r="X1" s="162"/>
-      <c r="Y1" s="162"/>
-      <c r="Z1" s="162"/>
-      <c r="AA1" s="162"/>
-      <c r="AB1" s="162"/>
-      <c r="AC1" s="162"/>
-      <c r="AD1" s="162"/>
-      <c r="AE1" s="162"/>
+      <c r="L1" s="175"/>
+      <c r="M1" s="175"/>
+      <c r="N1" s="175"/>
+      <c r="O1" s="175"/>
+      <c r="P1" s="175"/>
+      <c r="Q1" s="175"/>
+      <c r="R1" s="175"/>
+      <c r="S1" s="175"/>
+      <c r="T1" s="175"/>
+      <c r="U1" s="175"/>
+      <c r="V1" s="175"/>
+      <c r="W1" s="175"/>
+      <c r="X1" s="175"/>
+      <c r="Y1" s="175"/>
+      <c r="Z1" s="175"/>
+      <c r="AA1" s="175"/>
+      <c r="AB1" s="175"/>
+      <c r="AC1" s="175"/>
+      <c r="AD1" s="175"/>
+      <c r="AE1" s="175"/>
     </row>
     <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="51" t="s">
@@ -3951,11 +3951,11 @@
       <c r="B4" s="113" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="167">
+      <c r="C4" s="177">
         <v>45194</v>
       </c>
-      <c r="D4" s="167"/>
-      <c r="E4" s="167"/>
+      <c r="D4" s="177"/>
+      <c r="E4" s="177"/>
       <c r="F4" s="110"/>
       <c r="G4" s="113" t="s">
         <v>75</v>
@@ -3965,182 +3965,182 @@
       </c>
       <c r="I4" s="111"/>
       <c r="J4" s="49"/>
-      <c r="K4" s="164" t="str">
+      <c r="K4" s="169" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="L4" s="165"/>
-      <c r="M4" s="165"/>
-      <c r="N4" s="165"/>
-      <c r="O4" s="165"/>
-      <c r="P4" s="165"/>
-      <c r="Q4" s="166"/>
-      <c r="R4" s="164" t="str">
+      <c r="L4" s="170"/>
+      <c r="M4" s="170"/>
+      <c r="N4" s="170"/>
+      <c r="O4" s="170"/>
+      <c r="P4" s="170"/>
+      <c r="Q4" s="171"/>
+      <c r="R4" s="169" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="S4" s="165"/>
-      <c r="T4" s="165"/>
-      <c r="U4" s="165"/>
-      <c r="V4" s="165"/>
-      <c r="W4" s="165"/>
-      <c r="X4" s="166"/>
-      <c r="Y4" s="164" t="str">
+      <c r="S4" s="170"/>
+      <c r="T4" s="170"/>
+      <c r="U4" s="170"/>
+      <c r="V4" s="170"/>
+      <c r="W4" s="170"/>
+      <c r="X4" s="171"/>
+      <c r="Y4" s="169" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="Z4" s="165"/>
-      <c r="AA4" s="165"/>
-      <c r="AB4" s="165"/>
-      <c r="AC4" s="165"/>
-      <c r="AD4" s="165"/>
-      <c r="AE4" s="166"/>
-      <c r="AF4" s="164" t="str">
+      <c r="Z4" s="170"/>
+      <c r="AA4" s="170"/>
+      <c r="AB4" s="170"/>
+      <c r="AC4" s="170"/>
+      <c r="AD4" s="170"/>
+      <c r="AE4" s="171"/>
+      <c r="AF4" s="169" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AG4" s="165"/>
-      <c r="AH4" s="165"/>
-      <c r="AI4" s="165"/>
-      <c r="AJ4" s="165"/>
-      <c r="AK4" s="165"/>
-      <c r="AL4" s="166"/>
-      <c r="AM4" s="164" t="str">
+      <c r="AG4" s="170"/>
+      <c r="AH4" s="170"/>
+      <c r="AI4" s="170"/>
+      <c r="AJ4" s="170"/>
+      <c r="AK4" s="170"/>
+      <c r="AL4" s="171"/>
+      <c r="AM4" s="169" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AN4" s="165"/>
-      <c r="AO4" s="165"/>
-      <c r="AP4" s="165"/>
-      <c r="AQ4" s="165"/>
-      <c r="AR4" s="165"/>
-      <c r="AS4" s="166"/>
-      <c r="AT4" s="164" t="str">
+      <c r="AN4" s="170"/>
+      <c r="AO4" s="170"/>
+      <c r="AP4" s="170"/>
+      <c r="AQ4" s="170"/>
+      <c r="AR4" s="170"/>
+      <c r="AS4" s="171"/>
+      <c r="AT4" s="169" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AU4" s="165"/>
-      <c r="AV4" s="165"/>
-      <c r="AW4" s="165"/>
-      <c r="AX4" s="165"/>
-      <c r="AY4" s="165"/>
-      <c r="AZ4" s="166"/>
-      <c r="BA4" s="164" t="str">
+      <c r="AU4" s="170"/>
+      <c r="AV4" s="170"/>
+      <c r="AW4" s="170"/>
+      <c r="AX4" s="170"/>
+      <c r="AY4" s="170"/>
+      <c r="AZ4" s="171"/>
+      <c r="BA4" s="169" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="BB4" s="165"/>
-      <c r="BC4" s="165"/>
-      <c r="BD4" s="165"/>
-      <c r="BE4" s="165"/>
-      <c r="BF4" s="165"/>
-      <c r="BG4" s="166"/>
-      <c r="BH4" s="164" t="str">
+      <c r="BB4" s="170"/>
+      <c r="BC4" s="170"/>
+      <c r="BD4" s="170"/>
+      <c r="BE4" s="170"/>
+      <c r="BF4" s="170"/>
+      <c r="BG4" s="171"/>
+      <c r="BH4" s="169" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BI4" s="165"/>
-      <c r="BJ4" s="165"/>
-      <c r="BK4" s="165"/>
-      <c r="BL4" s="165"/>
-      <c r="BM4" s="165"/>
-      <c r="BN4" s="166"/>
+      <c r="BI4" s="170"/>
+      <c r="BJ4" s="170"/>
+      <c r="BK4" s="170"/>
+      <c r="BL4" s="170"/>
+      <c r="BM4" s="170"/>
+      <c r="BN4" s="171"/>
     </row>
     <row r="5" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="109"/>
       <c r="B5" s="113" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="163" t="s">
+      <c r="C5" s="176" t="s">
         <v>140</v>
       </c>
-      <c r="D5" s="163"/>
-      <c r="E5" s="163"/>
+      <c r="D5" s="176"/>
+      <c r="E5" s="176"/>
       <c r="F5" s="112"/>
       <c r="G5" s="112"/>
       <c r="H5" s="112"/>
       <c r="I5" s="112"/>
       <c r="J5" s="49"/>
-      <c r="K5" s="168">
+      <c r="K5" s="172">
         <f>K6</f>
         <v>45194</v>
       </c>
-      <c r="L5" s="169"/>
-      <c r="M5" s="169"/>
-      <c r="N5" s="169"/>
-      <c r="O5" s="169"/>
-      <c r="P5" s="169"/>
-      <c r="Q5" s="170"/>
-      <c r="R5" s="168">
+      <c r="L5" s="173"/>
+      <c r="M5" s="173"/>
+      <c r="N5" s="173"/>
+      <c r="O5" s="173"/>
+      <c r="P5" s="173"/>
+      <c r="Q5" s="174"/>
+      <c r="R5" s="172">
         <f>R6</f>
         <v>45201</v>
       </c>
-      <c r="S5" s="169"/>
-      <c r="T5" s="169"/>
-      <c r="U5" s="169"/>
-      <c r="V5" s="169"/>
-      <c r="W5" s="169"/>
-      <c r="X5" s="170"/>
-      <c r="Y5" s="168">
+      <c r="S5" s="173"/>
+      <c r="T5" s="173"/>
+      <c r="U5" s="173"/>
+      <c r="V5" s="173"/>
+      <c r="W5" s="173"/>
+      <c r="X5" s="174"/>
+      <c r="Y5" s="172">
         <f>Y6</f>
         <v>45208</v>
       </c>
-      <c r="Z5" s="169"/>
-      <c r="AA5" s="169"/>
-      <c r="AB5" s="169"/>
-      <c r="AC5" s="169"/>
-      <c r="AD5" s="169"/>
-      <c r="AE5" s="170"/>
-      <c r="AF5" s="168">
+      <c r="Z5" s="173"/>
+      <c r="AA5" s="173"/>
+      <c r="AB5" s="173"/>
+      <c r="AC5" s="173"/>
+      <c r="AD5" s="173"/>
+      <c r="AE5" s="174"/>
+      <c r="AF5" s="172">
         <f>AF6</f>
         <v>45215</v>
       </c>
-      <c r="AG5" s="169"/>
-      <c r="AH5" s="169"/>
-      <c r="AI5" s="169"/>
-      <c r="AJ5" s="169"/>
-      <c r="AK5" s="169"/>
-      <c r="AL5" s="170"/>
-      <c r="AM5" s="168">
+      <c r="AG5" s="173"/>
+      <c r="AH5" s="173"/>
+      <c r="AI5" s="173"/>
+      <c r="AJ5" s="173"/>
+      <c r="AK5" s="173"/>
+      <c r="AL5" s="174"/>
+      <c r="AM5" s="172">
         <f>AM6</f>
         <v>45222</v>
       </c>
-      <c r="AN5" s="169"/>
-      <c r="AO5" s="169"/>
-      <c r="AP5" s="169"/>
-      <c r="AQ5" s="169"/>
-      <c r="AR5" s="169"/>
-      <c r="AS5" s="170"/>
-      <c r="AT5" s="168">
+      <c r="AN5" s="173"/>
+      <c r="AO5" s="173"/>
+      <c r="AP5" s="173"/>
+      <c r="AQ5" s="173"/>
+      <c r="AR5" s="173"/>
+      <c r="AS5" s="174"/>
+      <c r="AT5" s="172">
         <f>AT6</f>
         <v>45229</v>
       </c>
-      <c r="AU5" s="169"/>
-      <c r="AV5" s="169"/>
-      <c r="AW5" s="169"/>
-      <c r="AX5" s="169"/>
-      <c r="AY5" s="169"/>
-      <c r="AZ5" s="170"/>
-      <c r="BA5" s="168">
+      <c r="AU5" s="173"/>
+      <c r="AV5" s="173"/>
+      <c r="AW5" s="173"/>
+      <c r="AX5" s="173"/>
+      <c r="AY5" s="173"/>
+      <c r="AZ5" s="174"/>
+      <c r="BA5" s="172">
         <f>BA6</f>
         <v>45236</v>
       </c>
-      <c r="BB5" s="169"/>
-      <c r="BC5" s="169"/>
-      <c r="BD5" s="169"/>
-      <c r="BE5" s="169"/>
-      <c r="BF5" s="169"/>
-      <c r="BG5" s="170"/>
-      <c r="BH5" s="168">
+      <c r="BB5" s="173"/>
+      <c r="BC5" s="173"/>
+      <c r="BD5" s="173"/>
+      <c r="BE5" s="173"/>
+      <c r="BF5" s="173"/>
+      <c r="BG5" s="174"/>
+      <c r="BH5" s="172">
         <f>BH6</f>
         <v>45243</v>
       </c>
-      <c r="BI5" s="169"/>
-      <c r="BJ5" s="169"/>
-      <c r="BK5" s="169"/>
-      <c r="BL5" s="169"/>
-      <c r="BM5" s="169"/>
-      <c r="BN5" s="170"/>
+      <c r="BI5" s="173"/>
+      <c r="BJ5" s="173"/>
+      <c r="BK5" s="173"/>
+      <c r="BL5" s="173"/>
+      <c r="BM5" s="173"/>
+      <c r="BN5" s="174"/>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A6" s="48"/>
@@ -5406,7 +5406,7 @@
     </row>
     <row r="17" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A17:A22" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.1</v>
       </c>
       <c r="B17" s="125" t="s">
@@ -5494,7 +5494,7 @@
     </row>
     <row r="18" spans="1:66" s="60" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A18" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" si="9"/>
         <v>3.2</v>
       </c>
       <c r="B18" s="125" t="s">
@@ -5582,7 +5582,7 @@
     </row>
     <row r="19" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" si="9"/>
         <v>3.3</v>
       </c>
       <c r="B19" s="125" t="s">
@@ -5670,7 +5670,7 @@
     </row>
     <row r="20" spans="1:66" s="60" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A20" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" si="9"/>
         <v>3.4</v>
       </c>
       <c r="B20" s="125" t="s">
@@ -5692,7 +5692,7 @@
         <v>1</v>
       </c>
       <c r="H20" s="62">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I20" s="63">
         <f t="shared" si="4"/>
@@ -5758,7 +5758,7 @@
     </row>
     <row r="21" spans="1:66" s="60" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A21" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" si="9"/>
         <v>3.5</v>
       </c>
       <c r="B21" s="125" t="s">
@@ -5846,7 +5846,7 @@
     </row>
     <row r="22" spans="1:66" s="60" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="59" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" si="9"/>
         <v>3.6</v>
       </c>
       <c r="B22" s="125" t="s">
@@ -5855,26 +5855,26 @@
       <c r="C22" s="60" t="s">
         <v>160</v>
       </c>
-      <c r="D22" s="172"/>
-      <c r="E22" s="173">
+      <c r="D22" s="162"/>
+      <c r="E22" s="163">
         <f>F20+1</f>
         <v>45210</v>
       </c>
-      <c r="F22" s="174">
+      <c r="F22" s="164">
         <f t="shared" si="6"/>
         <v>45210</v>
       </c>
-      <c r="G22" s="175">
+      <c r="G22" s="165">
         <v>1</v>
       </c>
-      <c r="H22" s="176">
+      <c r="H22" s="166">
         <v>0</v>
       </c>
-      <c r="I22" s="177">
+      <c r="I22" s="167">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="J22" s="178"/>
+      <c r="J22" s="168"/>
       <c r="K22" s="106"/>
       <c r="L22" s="106"/>
       <c r="M22" s="106"/>
@@ -6724,7 +6724,7 @@
       <c r="D33" s="78"/>
       <c r="E33" s="99"/>
       <c r="F33" s="100" t="str">
-        <f t="shared" ref="F33:F36" si="9">IF(ISBLANK(E33)," - ",IF(G33=0,E33,E33+G33-1))</f>
+        <f t="shared" ref="F33:F36" si="10">IF(ISBLANK(E33)," - ",IF(G33=0,E33,E33+G33-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G33" s="61"/>
@@ -6803,13 +6803,13 @@
       <c r="D34" s="78"/>
       <c r="E34" s="99"/>
       <c r="F34" s="100" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G34" s="61"/>
       <c r="H34" s="62"/>
       <c r="I34" s="79" t="str">
-        <f t="shared" ref="I34:I36" si="10">IF(OR(F34=0,E34=0)," - ",NETWORKDAYS(E34,F34))</f>
+        <f t="shared" ref="I34:I36" si="11">IF(OR(F34=0,E34=0)," - ",NETWORKDAYS(E34,F34))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J34" s="98"/>
@@ -6882,13 +6882,13 @@
       <c r="D35" s="78"/>
       <c r="E35" s="99"/>
       <c r="F35" s="100" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G35" s="61"/>
       <c r="H35" s="62"/>
       <c r="I35" s="79" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J35" s="98"/>
@@ -6961,13 +6961,13 @@
       <c r="D36" s="78"/>
       <c r="E36" s="99"/>
       <c r="F36" s="100" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G36" s="61"/>
       <c r="H36" s="62"/>
       <c r="I36" s="79" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J36" s="98"/>
@@ -7102,6 +7102,15 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -7112,15 +7121,6 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H8:H13 H15:H36">
@@ -7192,7 +7192,7 @@
   <pageSetup scale="63" fitToHeight="0" orientation="landscape" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
-    <ignoredError sqref="H9 A29:B30 B24 B25:B27 A32:B32 B31 E23 E29:H32 H12 H16 G23:H27 G33 G34:G35 G36 H18 H20" unlockedFormula="1"/>
+    <ignoredError sqref="H9 A29:B30 B24 B25:B27 A32:B32 B31 E23 E29:H32 H12 H16 G23:H27 G33 G34:G35 G36 H18" unlockedFormula="1"/>
     <ignoredError sqref="A23 A16 A12" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId3"/>
@@ -7524,10 +7524,10 @@
     </row>
     <row r="12" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A13" s="171" t="s">
+      <c r="A13" s="178" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="171"/>
+      <c r="B13" s="178"/>
     </row>
     <row r="14" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:3" s="132" customFormat="1" ht="18" x14ac:dyDescent="0.2">
@@ -7589,10 +7589,10 @@
       <c r="B23" s="10"/>
     </row>
     <row r="24" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A24" s="171" t="s">
+      <c r="A24" s="178" t="s">
         <v>87</v>
       </c>
-      <c r="B24" s="171"/>
+      <c r="B24" s="178"/>
     </row>
     <row r="25" spans="1:3" s="8" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A25" s="142"/>
@@ -7665,10 +7665,10 @@
       <c r="B37" s="10"/>
     </row>
     <row r="38" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A38" s="171" t="s">
+      <c r="A38" s="178" t="s">
         <v>11</v>
       </c>
-      <c r="B38" s="171"/>
+      <c r="B38" s="178"/>
     </row>
     <row r="39" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B39" s="139" t="s">
@@ -7705,10 +7705,10 @@
       <c r="B48" s="11"/>
     </row>
     <row r="49" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A49" s="171" t="s">
+      <c r="A49" s="178" t="s">
         <v>7</v>
       </c>
-      <c r="B49" s="171"/>
+      <c r="B49" s="178"/>
     </row>
     <row r="50" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B50" s="139" t="s">
@@ -7806,10 +7806,10 @@
       <c r="B64" s="12"/>
     </row>
     <row r="65" spans="1:2" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A65" s="171" t="s">
+      <c r="A65" s="178" t="s">
         <v>10</v>
       </c>
-      <c r="B65" s="171"/>
+      <c r="B65" s="178"/>
     </row>
     <row r="66" spans="1:2" s="20" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B66" s="139" t="s">
@@ -7820,10 +7820,10 @@
       <c r="B67" s="13"/>
     </row>
     <row r="68" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A68" s="171" t="s">
+      <c r="A68" s="178" t="s">
         <v>5</v>
       </c>
-      <c r="B68" s="171"/>
+      <c r="B68" s="178"/>
     </row>
     <row r="69" spans="1:2" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="154" t="s">

</xml_diff>